<commit_message>
New packet for 神將紅包
</commit_message>
<xml_diff>
--- a/PacketInfo/Sample.xlsx
+++ b/PacketInfo/Sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="515">
   <si>
     <t xml:space="preserve"> {"act":"Activity.drawCompanyAnniversaryLoginReward","sid":"3fc3b84cbd46610e7363daf513b792a962898752"}</t>
   </si>
@@ -1563,6 +1563,12 @@
   </si>
   <si>
     <t>getYunYouInfo</t>
+  </si>
+  <si>
+    <t>getShuangShiyiActivityReward</t>
+  </si>
+  <si>
+    <t>{"act":"Activity.getShuangShiyiActivityReward","sid":"3fc3b84cbd46610e7363daf533d182bd500440a7"}</t>
   </si>
 </sst>
 </file>
@@ -1578,12 +1584,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1598,8 +1610,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1914,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E232"/>
+  <dimension ref="A1:E233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,7 +1965,7 @@
         <v>296</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C65" si="0">CONCATENATE("private const string CMD_",B2," = """,A2,".",B2,""";")</f>
+        <f t="shared" ref="C2:C66" si="0">CONCATENATE("private const string CMD_",B2," = """,A2,".",B2,""";")</f>
         <v>private const string CMD_drawCompanyAnniversaryRechargeReward = "Activity.drawCompanyAnniversaryRechargeReward";</v>
       </c>
       <c r="E2" t="s">
@@ -2124,19 +2137,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B14" t="s">
-        <v>308</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>private const string CMD_getTuanGouOpenInfo = "Activity.getTuanGouOpenInfo";</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
+      <c r="B14" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>private const string CMD_getShuangShiyiActivityReward = "Activity.getShuangShiyiActivityReward";</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2144,14 +2157,14 @@
         <v>232</v>
       </c>
       <c r="B15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_serverOpenTime = "Activity.serverOpenTime";</v>
+        <v>private const string CMD_getTuanGouOpenInfo = "Activity.getTuanGouOpenInfo";</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2159,29 +2172,29 @@
         <v>232</v>
       </c>
       <c r="B16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_showIconForServerOpenActivity = "Activity.showIconForServerOpenActivity";</v>
+        <v>private const string CMD_serverOpenTime = "Activity.serverOpenTime";</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_archeryOpenInfo = "Archery.archeryOpenInfo";</v>
+        <v>private const string CMD_showIconForServerOpenActivity = "Activity.showIconForServerOpenActivity";</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2189,14 +2202,14 @@
         <v>233</v>
       </c>
       <c r="B18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getArcheryInfo = "Archery.getArcheryInfo";</v>
+        <v>private const string CMD_archeryOpenInfo = "Archery.archeryOpenInfo";</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2204,14 +2217,14 @@
         <v>233</v>
       </c>
       <c r="B19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getArcheryRewardInfo = "Archery.getArcheryRewardInfo";</v>
+        <v>private const string CMD_getArcheryInfo = "Archery.getArcheryInfo";</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2219,14 +2232,14 @@
         <v>233</v>
       </c>
       <c r="B20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getReward = "Archery.getReward";</v>
+        <v>private const string CMD_getArcheryRewardInfo = "Archery.getArcheryRewardInfo";</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2234,29 +2247,29 @@
         <v>233</v>
       </c>
       <c r="B21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_shoot = "Archery.shoot";</v>
+        <v>private const string CMD_getReward = "Archery.getReward";</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getBagInfo = "Bag.getBagInfo";</v>
+        <v>private const string CMD_shoot = "Archery.shoot";</v>
       </c>
       <c r="E22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2264,44 +2277,44 @@
         <v>234</v>
       </c>
       <c r="B23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_useItem = "Bag.useItem";</v>
+        <v>private const string CMD_getBagInfo = "Bag.getBagInfo";</v>
       </c>
       <c r="E23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getTimeInfo = "BaiGuanYu.getTimeInfo";</v>
+        <v>private const string CMD_useItem = "Bag.useItem";</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_bossInfo = "BossWar.bossInfo";</v>
+        <v>private const string CMD_getTimeInfo = "BaiGuanYu.getTimeInfo";</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2309,14 +2322,14 @@
         <v>236</v>
       </c>
       <c r="B26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_bossLineup = "BossWar.bossLineup";</v>
+        <v>private const string CMD_bossInfo = "BossWar.bossInfo";</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2324,14 +2337,14 @@
         <v>236</v>
       </c>
       <c r="B27" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_enterWar = "BossWar.enterWar";</v>
+        <v>private const string CMD_bossLineup = "BossWar.bossLineup";</v>
       </c>
       <c r="E27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2339,14 +2352,14 @@
         <v>236</v>
       </c>
       <c r="B28" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_keyKillInfo = "BossWar.keyKillInfo";</v>
+        <v>private const string CMD_enterWar = "BossWar.enterWar";</v>
       </c>
       <c r="E28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2354,14 +2367,14 @@
         <v>236</v>
       </c>
       <c r="B29" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_leaveWar = "BossWar.leaveWar";</v>
+        <v>private const string CMD_keyKillInfo = "BossWar.keyKillInfo";</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2369,14 +2382,14 @@
         <v>236</v>
       </c>
       <c r="B30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_openInfo = "BossWar.openInfo";</v>
+        <v>private const string CMD_leaveWar = "BossWar.leaveWar";</v>
       </c>
       <c r="E30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2384,14 +2397,14 @@
         <v>236</v>
       </c>
       <c r="B31" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_pk = "BossWar.pk";</v>
+        <v>private const string CMD_openInfo = "BossWar.openInfo";</v>
       </c>
       <c r="E31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2399,14 +2412,14 @@
         <v>236</v>
       </c>
       <c r="B32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_rankInfo = "BossWar.rankInfo";</v>
+        <v>private const string CMD_pk = "BossWar.pk";</v>
       </c>
       <c r="E32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2414,29 +2427,29 @@
         <v>236</v>
       </c>
       <c r="B33" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_sendTroop = "BossWar.sendTroop";</v>
+        <v>private const string CMD_rankInfo = "BossWar.rankInfo";</v>
       </c>
       <c r="E33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_eliteBuyTime = "Campaign.eliteBuyTime";</v>
+        <v>private const string CMD_sendTroop = "BossWar.sendTroop";</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2444,14 +2457,14 @@
         <v>237</v>
       </c>
       <c r="B35" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_eliteFight = "Campaign.eliteFight";</v>
+        <v>private const string CMD_eliteBuyTime = "Campaign.eliteBuyTime";</v>
       </c>
       <c r="E35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2459,14 +2472,14 @@
         <v>237</v>
       </c>
       <c r="B36" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_eliteGetAllInfos = "Campaign.eliteGetAllInfos";</v>
+        <v>private const string CMD_eliteFight = "Campaign.eliteFight";</v>
       </c>
       <c r="E36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2474,14 +2487,14 @@
         <v>237</v>
       </c>
       <c r="B37" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_eliteGetCampaignInfo = "Campaign.eliteGetCampaignInfo";</v>
+        <v>private const string CMD_eliteGetAllInfos = "Campaign.eliteGetAllInfos";</v>
       </c>
       <c r="E37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2489,14 +2502,14 @@
         <v>237</v>
       </c>
       <c r="B38" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_evalMarchFormation = "Campaign.evalMarchFormation";</v>
+        <v>private const string CMD_eliteGetCampaignInfo = "Campaign.eliteGetCampaignInfo";</v>
       </c>
       <c r="E38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2504,14 +2517,14 @@
         <v>237</v>
       </c>
       <c r="B39" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_fightNext = "Campaign.fightNext";</v>
+        <v>private const string CMD_evalMarchFormation = "Campaign.evalMarchFormation";</v>
       </c>
       <c r="E39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2519,14 +2532,14 @@
         <v>237</v>
       </c>
       <c r="B40" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getAttFormation = "Campaign.getAttFormation";</v>
+        <v>private const string CMD_fightNext = "Campaign.fightNext";</v>
       </c>
       <c r="E40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2534,14 +2547,14 @@
         <v>237</v>
       </c>
       <c r="B41" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getLeftTimes = "Campaign.getLeftTimes";</v>
+        <v>private const string CMD_getAttFormation = "Campaign.getAttFormation";</v>
       </c>
       <c r="E41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2549,14 +2562,14 @@
         <v>237</v>
       </c>
       <c r="B42" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getTrialsInfo = "Campaign.getTrialsInfo";</v>
+        <v>private const string CMD_getLeftTimes = "Campaign.getLeftTimes";</v>
       </c>
       <c r="E42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2564,14 +2577,14 @@
         <v>237</v>
       </c>
       <c r="B43" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_nextEnemies = "Campaign.nextEnemies";</v>
+        <v>private const string CMD_getTrialsInfo = "Campaign.getTrialsInfo";</v>
       </c>
       <c r="E43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2579,14 +2592,14 @@
         <v>237</v>
       </c>
       <c r="B44" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_quitCampaign = "Campaign.quitCampaign";</v>
+        <v>private const string CMD_nextEnemies = "Campaign.nextEnemies";</v>
       </c>
       <c r="E44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2594,14 +2607,14 @@
         <v>237</v>
       </c>
       <c r="B45" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_saveFormation = "Campaign.saveFormation";</v>
+        <v>private const string CMD_quitCampaign = "Campaign.quitCampaign";</v>
       </c>
       <c r="E45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2609,44 +2622,44 @@
         <v>237</v>
       </c>
       <c r="B46" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_trialsBuyTimes = "Campaign.trialsBuyTimes";</v>
+        <v>private const string CMD_saveFormation = "Campaign.saveFormation";</v>
       </c>
       <c r="E46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B47" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_time = "ChristmasTree.time";</v>
+        <v>private const string CMD_trialsBuyTimes = "Campaign.trialsBuyTimes";</v>
       </c>
       <c r="E47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_challenge = "Circle.challenge";</v>
+        <v>private const string CMD_time = "ChristmasTree.time";</v>
       </c>
       <c r="E48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2654,14 +2667,14 @@
         <v>239</v>
       </c>
       <c r="B49" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_drawPassRewards = "Circle.drawPassRewards";</v>
+        <v>private const string CMD_challenge = "Circle.challenge";</v>
       </c>
       <c r="E49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2669,14 +2682,14 @@
         <v>239</v>
       </c>
       <c r="B50" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getHuarongRoadInfo = "Circle.getHuarongRoadInfo";</v>
+        <v>private const string CMD_drawPassRewards = "Circle.drawPassRewards";</v>
       </c>
       <c r="E50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2684,14 +2697,14 @@
         <v>239</v>
       </c>
       <c r="B51" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_restartHuarongRoad = "Circle.restartHuarongRoad";</v>
+        <v>private const string CMD_getHuarongRoadInfo = "Circle.getHuarongRoadInfo";</v>
       </c>
       <c r="E51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2699,29 +2712,29 @@
         <v>239</v>
       </c>
       <c r="B52" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_turnOverHeroCard = "Circle.turnOverHeroCard";</v>
+        <v>private const string CMD_restartHuarongRoad = "Circle.restartHuarongRoad";</v>
       </c>
       <c r="E52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B53" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_buyProduct = "City.buyProduct";</v>
+        <v>private const string CMD_turnOverHeroCard = "Circle.turnOverHeroCard";</v>
       </c>
       <c r="E53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2729,14 +2742,14 @@
         <v>240</v>
       </c>
       <c r="B54" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getIndustryInfo = "City.getIndustryInfo";</v>
+        <v>private const string CMD_buyProduct = "City.buyProduct";</v>
       </c>
       <c r="E54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2744,29 +2757,29 @@
         <v>240</v>
       </c>
       <c r="B55" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getPlayerCityInfo = "City.getPlayerCityInfo";</v>
+        <v>private const string CMD_getIndustryInfo = "City.getIndustryInfo";</v>
       </c>
       <c r="E55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B56" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_corpsCityReward = "Corps.corpsCityReward";</v>
+        <v>private const string CMD_getPlayerCityInfo = "City.getPlayerCityInfo";</v>
       </c>
       <c r="E56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2774,14 +2787,14 @@
         <v>241</v>
       </c>
       <c r="B57" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getCityRewardInfo = "Corps.getCityRewardInfo";</v>
+        <v>private const string CMD_corpsCityReward = "Corps.corpsCityReward";</v>
       </c>
       <c r="E57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2789,14 +2802,14 @@
         <v>241</v>
       </c>
       <c r="B58" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getCorpsJoinedPlayers = "Corps.getCorpsJoinedPlayers";</v>
+        <v>private const string CMD_getCityRewardInfo = "Corps.getCityRewardInfo";</v>
       </c>
       <c r="E58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2804,14 +2817,14 @@
         <v>241</v>
       </c>
       <c r="B59" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getCorpsMessageNum = "Corps.getCorpsMessageNum";</v>
+        <v>private const string CMD_getCorpsJoinedPlayers = "Corps.getCorpsJoinedPlayers";</v>
       </c>
       <c r="E59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2819,14 +2832,14 @@
         <v>241</v>
       </c>
       <c r="B60" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getJoinedCorps = "Corps.getJoinedCorps";</v>
+        <v>private const string CMD_getCorpsMessageNum = "Corps.getCorpsMessageNum";</v>
       </c>
       <c r="E60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2834,14 +2847,14 @@
         <v>241</v>
       </c>
       <c r="B61" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_getNationalRank = "Corps.getNationalRank";</v>
+        <v>private const string CMD_getJoinedCorps = "Corps.getJoinedCorps";</v>
       </c>
       <c r="E61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2849,14 +2862,14 @@
         <v>241</v>
       </c>
       <c r="B62" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_personIndustryList = "Corps.personIndustryList";</v>
+        <v>private const string CMD_getNationalRank = "Corps.getNationalRank";</v>
       </c>
       <c r="E62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,14 +2877,14 @@
         <v>241</v>
       </c>
       <c r="B63" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_personIndustryRefresh = "Corps.personIndustryRefresh";</v>
+        <v>private const string CMD_personIndustryList = "Corps.personIndustryList";</v>
       </c>
       <c r="E63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2879,14 +2892,14 @@
         <v>241</v>
       </c>
       <c r="B64" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_playerTech = "Corps.playerTech";</v>
+        <v>private const string CMD_personIndustryRefresh = "Corps.personIndustryRefresh";</v>
       </c>
       <c r="E64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2894,14 +2907,14 @@
         <v>241</v>
       </c>
       <c r="B65" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
-        <v>private const string CMD_takeZhanjiStep = "Corps.takeZhanjiStep";</v>
+        <v>private const string CMD_playerTech = "Corps.playerTech";</v>
       </c>
       <c r="E65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2909,44 +2922,44 @@
         <v>241</v>
       </c>
       <c r="B66" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C129" si="1">CONCATENATE("private const string CMD_",B66," = """,A66,".",B66,""";")</f>
-        <v>private const string CMD_upgradePlayerTech = "Corps.upgradePlayerTech";</v>
+        <f t="shared" si="0"/>
+        <v>private const string CMD_takeZhanjiStep = "Corps.takeZhanjiStep";</v>
       </c>
       <c r="E66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B67" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="1"/>
-        <v>private const string CMD_getInfo = "CorpsWar.getInfo";</v>
+        <f t="shared" ref="C67:C130" si="1">CONCATENATE("private const string CMD_",B67," = """,A67,".",B67,""";")</f>
+        <v>private const string CMD_upgradePlayerTech = "Corps.upgradePlayerTech";</v>
       </c>
       <c r="E67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B68" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_corpsCountry = "Country.corpsCountry";</v>
+        <v>private const string CMD_getInfo = "CorpsWar.getInfo";</v>
       </c>
       <c r="E68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2954,29 +2967,29 @@
         <v>243</v>
       </c>
       <c r="B69" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_viewCountry = "Country.viewCountry";</v>
+        <v>private const string CMD_corpsCountry = "Country.corpsCountry";</v>
       </c>
       <c r="E69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B70" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getInfo = "CrossCamp.getInfo";</v>
+        <v>private const string CMD_viewCountry = "Country.viewCountry";</v>
       </c>
       <c r="E70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2984,59 +2997,59 @@
         <v>244</v>
       </c>
       <c r="B71" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getJackpotInfo = "CrossCamp.getJackpotInfo";</v>
+        <v>private const string CMD_getInfo = "CrossCamp.getInfo";</v>
       </c>
       <c r="E71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B72" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getCurrActivityInfo = "DaqiaoActivity.getCurrActivityInfo";</v>
+        <v>private const string CMD_getJackpotInfo = "CrossCamp.getJackpotInfo";</v>
       </c>
       <c r="E72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B73" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getDramaInfo = "Drama.getDramaInfo";</v>
+        <v>private const string CMD_getCurrActivityInfo = "DaqiaoActivity.getCurrActivityInfo";</v>
       </c>
       <c r="E73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B74" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_attack = "EightTrigrams.attack";</v>
+        <v>private const string CMD_getDramaInfo = "Drama.getDramaInfo";</v>
       </c>
       <c r="E74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3044,14 +3057,14 @@
         <v>247</v>
       </c>
       <c r="B75" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getInfo = "EightTrigrams.getInfo";</v>
+        <v>private const string CMD_attack = "EightTrigrams.attack";</v>
       </c>
       <c r="E75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3059,14 +3072,14 @@
         <v>247</v>
       </c>
       <c r="B76" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_open = "EightTrigrams.open";</v>
+        <v>private const string CMD_getInfo = "EightTrigrams.getInfo";</v>
       </c>
       <c r="E76" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3074,29 +3087,29 @@
         <v>247</v>
       </c>
       <c r="B77" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_openBox = "EightTrigrams.openBox";</v>
+        <v>private const string CMD_open = "EightTrigrams.open";</v>
       </c>
       <c r="E77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B78" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getAttachment = "Email.getAttachment";</v>
+        <v>private const string CMD_openBox = "EightTrigrams.openBox";</v>
       </c>
       <c r="E78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3104,14 +3117,14 @@
         <v>248</v>
       </c>
       <c r="B79" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_openInBox = "Email.openInBox";</v>
+        <v>private const string CMD_getAttachment = "Email.getAttachment";</v>
       </c>
       <c r="E79" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3119,29 +3132,29 @@
         <v>248</v>
       </c>
       <c r="B80" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_read = "Email.read";</v>
+        <v>private const string CMD_openInBox = "Email.openInBox";</v>
       </c>
       <c r="E80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B81" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_collect = "Emperor.collect";</v>
+        <v>private const string CMD_read = "Email.read";</v>
       </c>
       <c r="E81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3149,14 +3162,14 @@
         <v>249</v>
       </c>
       <c r="B82" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_collected = "Emperor.collected";</v>
+        <v>private const string CMD_collect = "Emperor.collect";</v>
       </c>
       <c r="E82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3164,14 +3177,14 @@
         <v>249</v>
       </c>
       <c r="B83" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_draw = "Emperor.draw";</v>
+        <v>private const string CMD_collected = "Emperor.collected";</v>
       </c>
       <c r="E83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3179,14 +3192,14 @@
         <v>249</v>
       </c>
       <c r="B84" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getBuyInfo = "Emperor.getBuyInfo";</v>
+        <v>private const string CMD_draw = "Emperor.draw";</v>
       </c>
       <c r="E84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3194,14 +3207,14 @@
         <v>249</v>
       </c>
       <c r="B85" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getGameInfo = "Emperor.getGameInfo";</v>
+        <v>private const string CMD_getBuyInfo = "Emperor.getBuyInfo";</v>
       </c>
       <c r="E85" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3209,29 +3222,29 @@
         <v>249</v>
       </c>
       <c r="B86" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_isFloat = "Emperor.isFloat";</v>
+        <v>private const string CMD_getGameInfo = "Emperor.getGameInfo";</v>
       </c>
       <c r="E86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B87" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_activityInfo = "Firecracker.activityInfo";</v>
+        <v>private const string CMD_isFloat = "Emperor.isFloat";</v>
       </c>
       <c r="E87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3239,59 +3252,59 @@
         <v>250</v>
       </c>
       <c r="B88" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_myFirecrackerInfo = "Firecracker.myFirecrackerInfo";</v>
+        <v>private const string CMD_activityInfo = "Firecracker.activityInfo";</v>
       </c>
       <c r="E88" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B89" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_chouqianOpenInfo = "Gamble.chouqianOpenInfo";</v>
+        <v>private const string CMD_myFirecrackerInfo = "Firecracker.myFirecrackerInfo";</v>
       </c>
       <c r="E89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B90" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_superPackageInfo = "GmActivity.superPackageInfo";</v>
+        <v>private const string CMD_chouqianOpenInfo = "Gamble.chouqianOpenInfo";</v>
       </c>
       <c r="E90" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B91" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_godActToStren = "God.godActToStren";</v>
+        <v>private const string CMD_superPackageInfo = "GmActivity.superPackageInfo";</v>
       </c>
       <c r="E91" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3299,14 +3312,14 @@
         <v>253</v>
       </c>
       <c r="B92" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_godStrenInfo = "God.godStrenInfo";</v>
+        <v>private const string CMD_godActToStren = "God.godActToStren";</v>
       </c>
       <c r="E92" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3314,29 +3327,29 @@
         <v>253</v>
       </c>
       <c r="B93" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_godStrenOrAdvance = "God.godStrenOrAdvance";</v>
+        <v>private const string CMD_godStrenInfo = "God.godStrenInfo";</v>
       </c>
       <c r="E93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B94" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_acquireGrassArrowInfo = "GrassArrow.acquireGrassArrowInfo";</v>
+        <v>private const string CMD_godStrenOrAdvance = "God.godStrenOrAdvance";</v>
       </c>
       <c r="E94" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3344,14 +3357,14 @@
         <v>254</v>
       </c>
       <c r="B95" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_doGrassArrowFight = "GrassArrow.doGrassArrowFight";</v>
+        <v>private const string CMD_acquireGrassArrowInfo = "GrassArrow.acquireGrassArrowInfo";</v>
       </c>
       <c r="E95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3359,14 +3372,14 @@
         <v>254</v>
       </c>
       <c r="B96" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_drawStageReward = "GrassArrow.drawStageReward";</v>
+        <v>private const string CMD_doGrassArrowFight = "GrassArrow.doGrassArrowFight";</v>
       </c>
       <c r="E96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3374,29 +3387,29 @@
         <v>254</v>
       </c>
       <c r="B97" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_exchangeGrassArrow = "GrassArrow.exchangeGrassArrow";</v>
+        <v>private const string CMD_drawStageReward = "GrassArrow.drawStageReward";</v>
       </c>
       <c r="E97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B98" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_assessScore = "Hero.assessScore";</v>
+        <v>private const string CMD_exchangeGrassArrow = "GrassArrow.exchangeGrassArrow";</v>
       </c>
       <c r="E98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3404,14 +3417,14 @@
         <v>255</v>
       </c>
       <c r="B99" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getConvenientFormations = "Hero.getConvenientFormations";</v>
+        <v>private const string CMD_assessScore = "Hero.assessScore";</v>
       </c>
       <c r="E99" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3419,14 +3432,14 @@
         <v>255</v>
       </c>
       <c r="B100" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getCurrRecommendActivityInfo = "Hero.getCurrRecommendActivityInfo";</v>
+        <v>private const string CMD_getConvenientFormations = "Hero.getConvenientFormations";</v>
       </c>
       <c r="E100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3434,14 +3447,14 @@
         <v>255</v>
       </c>
       <c r="B101" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getFeastInfo = "Hero.getFeastInfo";</v>
+        <v>private const string CMD_getCurrRecommendActivityInfo = "Hero.getCurrRecommendActivityInfo";</v>
       </c>
       <c r="E101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3449,14 +3462,14 @@
         <v>255</v>
       </c>
       <c r="B102" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getHeroIconInfo = "Hero.getHeroIconInfo";</v>
+        <v>private const string CMD_getFeastInfo = "Hero.getFeastInfo";</v>
       </c>
       <c r="E102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3464,14 +3477,14 @@
         <v>255</v>
       </c>
       <c r="B103" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getPlayerHeroList = "Hero.getPlayerHeroList";</v>
+        <v>private const string CMD_getHeroIconInfo = "Hero.getHeroIconInfo";</v>
       </c>
       <c r="E103" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3479,14 +3492,14 @@
         <v>255</v>
       </c>
       <c r="B104" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getScoreHero = "Hero.getScoreHero";</v>
+        <v>private const string CMD_getPlayerHeroList = "Hero.getPlayerHeroList";</v>
       </c>
       <c r="E104" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3494,14 +3507,14 @@
         <v>255</v>
       </c>
       <c r="B105" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getVisitHeroInfo = "Hero.getVisitHeroInfo";</v>
+        <v>private const string CMD_getScoreHero = "Hero.getScoreHero";</v>
       </c>
       <c r="E105" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3509,14 +3522,14 @@
         <v>255</v>
       </c>
       <c r="B106" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getWineInfo = "Hero.getWineInfo";</v>
+        <v>private const string CMD_getVisitHeroInfo = "Hero.getVisitHeroInfo";</v>
       </c>
       <c r="E106" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3524,29 +3537,29 @@
         <v>255</v>
       </c>
       <c r="B107" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_matchHero = "Hero.matchHero";</v>
+        <v>private const string CMD_getWineInfo = "Hero.getWineInfo";</v>
       </c>
       <c r="E107" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B108" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_afterSeasonEnemy = "KingRoad.afterSeasonEnemy";</v>
+        <v>private const string CMD_matchHero = "Hero.matchHero";</v>
       </c>
       <c r="E108" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3554,14 +3567,14 @@
         <v>256</v>
       </c>
       <c r="B109" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_kingroadEnd = "KingRoad.kingroadEnd";</v>
+        <v>private const string CMD_afterSeasonEnemy = "KingRoad.afterSeasonEnemy";</v>
       </c>
       <c r="E109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3569,14 +3582,14 @@
         <v>256</v>
       </c>
       <c r="B110" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_kingroadState = "KingRoad.kingroadState";</v>
+        <v>private const string CMD_kingroadEnd = "KingRoad.kingroadEnd";</v>
       </c>
       <c r="E110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3584,29 +3597,29 @@
         <v>256</v>
       </c>
       <c r="B111" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_seasonChallenge = "KingRoad.seasonChallenge";</v>
+        <v>private const string CMD_kingroadState = "KingRoad.kingroadState";</v>
       </c>
       <c r="E111" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B112" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getOfflineConpensate = "Login.getOfflineConpensate";</v>
+        <v>private const string CMD_seasonChallenge = "KingRoad.seasonChallenge";</v>
       </c>
       <c r="E112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3614,14 +3627,14 @@
         <v>257</v>
       </c>
       <c r="B113" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C113" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_login = "Login.login";</v>
+        <v>private const string CMD_getOfflineConpensate = "Login.getOfflineConpensate";</v>
       </c>
       <c r="E113" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3629,14 +3642,14 @@
         <v>257</v>
       </c>
       <c r="B114" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_loginFinish = "Login.loginFinish";</v>
+        <v>private const string CMD_login = "Login.login";</v>
       </c>
       <c r="E114" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3644,29 +3657,29 @@
         <v>257</v>
       </c>
       <c r="B115" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_serverInfo = "Login.serverInfo";</v>
+        <v>private const string CMD_loginFinish = "Login.loginFinish";</v>
       </c>
       <c r="E115" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B116" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getBuyResetTimes = "LongMarch.getBuyResetTimes";</v>
+        <v>private const string CMD_serverInfo = "Login.serverInfo";</v>
       </c>
       <c r="E116" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3674,14 +3687,14 @@
         <v>258</v>
       </c>
       <c r="B117" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getFinishedReward = "LongMarch.getFinishedReward";</v>
+        <v>private const string CMD_getBuyResetTimes = "LongMarch.getBuyResetTimes";</v>
       </c>
       <c r="E117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3689,14 +3702,14 @@
         <v>258</v>
       </c>
       <c r="B118" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getHeroStatus = "LongMarch.getHeroStatus";</v>
+        <v>private const string CMD_getFinishedReward = "LongMarch.getFinishedReward";</v>
       </c>
       <c r="E118" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3704,14 +3717,14 @@
         <v>258</v>
       </c>
       <c r="B119" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getMyStatus = "LongMarch.getMyStatus";</v>
+        <v>private const string CMD_getHeroStatus = "LongMarch.getHeroStatus";</v>
       </c>
       <c r="E119" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3719,14 +3732,14 @@
         <v>258</v>
       </c>
       <c r="B120" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C120" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getUnpassBuff = "LongMarch.getUnpassBuff";</v>
+        <v>private const string CMD_getMyStatus = "LongMarch.getMyStatus";</v>
       </c>
       <c r="E120" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3734,44 +3747,44 @@
         <v>258</v>
       </c>
       <c r="B121" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_restart = "LongMarch.restart";</v>
+        <v>private const string CMD_getUnpassBuff = "LongMarch.getUnpassBuff";</v>
       </c>
       <c r="E121" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B122" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getDispInfo = "LordGodUp.getDispInfo";</v>
+        <v>private const string CMD_restart = "LongMarch.restart";</v>
       </c>
       <c r="E122" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B123" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_drawLottery = "Lottery.drawLottery";</v>
+        <v>private const string CMD_getDispInfo = "LordGodUp.getDispInfo";</v>
       </c>
       <c r="E123" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3779,14 +3792,14 @@
         <v>260</v>
       </c>
       <c r="B124" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_freeLottery = "Lottery.freeLottery";</v>
+        <v>private const string CMD_drawLottery = "Lottery.drawLottery";</v>
       </c>
       <c r="E124" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -3794,14 +3807,14 @@
         <v>260</v>
       </c>
       <c r="B125" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C125" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_openLottery = "Lottery.openLottery";</v>
+        <v>private const string CMD_freeLottery = "Lottery.freeLottery";</v>
       </c>
       <c r="E125" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3809,29 +3822,29 @@
         <v>260</v>
       </c>
       <c r="B126" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C126" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_refreshLottery = "Lottery.refreshLottery";</v>
+        <v>private const string CMD_openLottery = "Lottery.openLottery";</v>
       </c>
       <c r="E126" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B127" t="s">
-        <v>375</v>
+        <v>418</v>
       </c>
       <c r="C127" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_draw = "LuckyCycle.draw";</v>
+        <v>private const string CMD_refreshLottery = "Lottery.refreshLottery";</v>
       </c>
       <c r="E127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3839,44 +3852,44 @@
         <v>261</v>
       </c>
       <c r="B128" t="s">
-        <v>419</v>
+        <v>375</v>
       </c>
       <c r="C128" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_info = "LuckyCycle.info";</v>
+        <v>private const string CMD_draw = "LuckyCycle.draw";</v>
       </c>
       <c r="E128" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B129" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C129" t="str">
         <f t="shared" si="1"/>
-        <v>private const string CMD_getMyMajorInfo = "Major.getMyMajorInfo";</v>
+        <v>private const string CMD_info = "LuckyCycle.info";</v>
       </c>
       <c r="E129" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B130" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C130" t="str">
-        <f t="shared" ref="C130:C193" si="2">CONCATENATE("private const string CMD_",B130," = """,A130,".",B130,""";")</f>
-        <v>private const string CMD_appointHero = "Manor.appointHero";</v>
+        <f t="shared" si="1"/>
+        <v>private const string CMD_getMyMajorInfo = "Major.getMyMajorInfo";</v>
       </c>
       <c r="E130" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3884,14 +3897,14 @@
         <v>263</v>
       </c>
       <c r="B131" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C131" t="str">
-        <f t="shared" si="2"/>
-        <v>private const string CMD_appointInfo = "Manor.appointInfo";</v>
+        <f t="shared" ref="C131:C194" si="2">CONCATENATE("private const string CMD_",B131," = """,A131,".",B131,""";")</f>
+        <v>private const string CMD_appointHero = "Manor.appointHero";</v>
       </c>
       <c r="E131" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3899,14 +3912,14 @@
         <v>263</v>
       </c>
       <c r="B132" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C132" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_armsTechnology = "Manor.armsTechnology";</v>
+        <v>private const string CMD_appointInfo = "Manor.appointInfo";</v>
       </c>
       <c r="E132" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3914,14 +3927,14 @@
         <v>263</v>
       </c>
       <c r="B133" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C133" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_autoAppoint = "Manor.autoAppoint";</v>
+        <v>private const string CMD_armsTechnology = "Manor.armsTechnology";</v>
       </c>
       <c r="E133" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3929,14 +3942,14 @@
         <v>263</v>
       </c>
       <c r="B134" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C134" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_currIncEffect = "Manor.currIncEffect";</v>
+        <v>private const string CMD_autoAppoint = "Manor.autoAppoint";</v>
       </c>
       <c r="E134" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3944,14 +3957,14 @@
         <v>263</v>
       </c>
       <c r="B135" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C135" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_decreeInfo = "Manor.decreeInfo";</v>
+        <v>private const string CMD_currIncEffect = "Manor.currIncEffect";</v>
       </c>
       <c r="E135" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3959,14 +3972,14 @@
         <v>263</v>
       </c>
       <c r="B136" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C136" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_doHeroActivity = "Manor.doHeroActivity";</v>
+        <v>private const string CMD_decreeInfo = "Manor.decreeInfo";</v>
       </c>
       <c r="E136" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3974,14 +3987,14 @@
         <v>263</v>
       </c>
       <c r="B137" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C137" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getManorInfo = "Manor.getManorInfo";</v>
+        <v>private const string CMD_doHeroActivity = "Manor.doHeroActivity";</v>
       </c>
       <c r="E137" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3989,14 +4002,14 @@
         <v>263</v>
       </c>
       <c r="B138" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C138" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_harvestActivity = "Manor.harvestActivity";</v>
+        <v>private const string CMD_getManorInfo = "Manor.getManorInfo";</v>
       </c>
       <c r="E138" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4004,14 +4017,14 @@
         <v>263</v>
       </c>
       <c r="B139" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C139" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_harvestProduct = "Manor.harvestProduct";</v>
+        <v>private const string CMD_harvestActivity = "Manor.harvestActivity";</v>
       </c>
       <c r="E139" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4019,14 +4032,14 @@
         <v>263</v>
       </c>
       <c r="B140" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C140" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_heroScoreTips = "Manor.heroScoreTips";</v>
+        <v>private const string CMD_harvestProduct = "Manor.harvestProduct";</v>
       </c>
       <c r="E140" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4034,14 +4047,14 @@
         <v>263</v>
       </c>
       <c r="B141" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C141" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_moveBuilding = "Manor.moveBuilding";</v>
+        <v>private const string CMD_heroScoreTips = "Manor.heroScoreTips";</v>
       </c>
       <c r="E141" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4049,14 +4062,14 @@
         <v>263</v>
       </c>
       <c r="B142" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C142" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_produceArmamentInfo = "Manor.produceArmamentInfo";</v>
+        <v>private const string CMD_moveBuilding = "Manor.moveBuilding";</v>
       </c>
       <c r="E142" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4064,14 +4077,14 @@
         <v>263</v>
       </c>
       <c r="B143" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C143" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_refreshManor = "Manor.refreshManor";</v>
+        <v>private const string CMD_produceArmamentInfo = "Manor.produceArmamentInfo";</v>
       </c>
       <c r="E143" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4079,14 +4092,14 @@
         <v>263</v>
       </c>
       <c r="B144" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C144" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_resHourOutput = "Manor.resHourOutput";</v>
+        <v>private const string CMD_refreshManor = "Manor.refreshManor";</v>
       </c>
       <c r="E144" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4094,14 +4107,14 @@
         <v>263</v>
       </c>
       <c r="B145" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C145" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_retireAll = "Manor.retireAll";</v>
+        <v>private const string CMD_resHourOutput = "Manor.resHourOutput";</v>
       </c>
       <c r="E145" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4109,14 +4122,14 @@
         <v>263</v>
       </c>
       <c r="B146" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C146" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_trainHeroInfo = "Manor.trainHeroInfo";</v>
+        <v>private const string CMD_retireAll = "Manor.retireAll";</v>
       </c>
       <c r="E146" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4124,44 +4137,44 @@
         <v>263</v>
       </c>
       <c r="B147" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C147" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_upgradeArmsTechnology = "Manor.upgradeArmsTechnology";</v>
+        <v>private const string CMD_trainHeroInfo = "Manor.trainHeroInfo";</v>
       </c>
       <c r="E147" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B148" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C148" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getOpenInfo = "MonthSignIn.getOpenInfo";</v>
+        <v>private const string CMD_upgradeArmsTechnology = "Manor.upgradeArmsTechnology";</v>
       </c>
       <c r="E148" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B149" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C149" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_acquireCityCommandInfo = "NationalWar.acquireCityCommandInfo";</v>
+        <v>private const string CMD_getOpenInfo = "MonthSignIn.getOpenInfo";</v>
       </c>
       <c r="E149" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4169,14 +4182,14 @@
         <v>265</v>
       </c>
       <c r="B150" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C150" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_acquireNationCardPanelInfo = "NationalWar.acquireNationCardPanelInfo";</v>
+        <v>private const string CMD_acquireCityCommandInfo = "NationalWar.acquireCityCommandInfo";</v>
       </c>
       <c r="E150" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4184,14 +4197,14 @@
         <v>265</v>
       </c>
       <c r="B151" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C151" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_cityDeclareInfo = "NationalWar.cityDeclareInfo";</v>
+        <v>private const string CMD_acquireNationCardPanelInfo = "NationalWar.acquireNationCardPanelInfo";</v>
       </c>
       <c r="E151" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4199,14 +4212,14 @@
         <v>265</v>
       </c>
       <c r="B152" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C152" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_convertNationCardReward = "NationalWar.convertNationCardReward";</v>
+        <v>private const string CMD_cityDeclareInfo = "NationalWar.cityDeclareInfo";</v>
       </c>
       <c r="E152" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4214,29 +4227,29 @@
         <v>265</v>
       </c>
       <c r="B153" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C153" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getMyTroops = "NationalWar.getMyTroops";</v>
+        <v>private const string CMD_convertNationCardReward = "NationalWar.convertNationCardReward";</v>
       </c>
       <c r="E153" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B154" t="s">
-        <v>321</v>
+        <v>444</v>
       </c>
       <c r="C154" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_enterWar = "Naval.enterWar";</v>
+        <v>private const string CMD_getMyTroops = "NationalWar.getMyTroops";</v>
       </c>
       <c r="E154" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4244,14 +4257,14 @@
         <v>266</v>
       </c>
       <c r="B155" t="s">
-        <v>361</v>
+        <v>321</v>
       </c>
       <c r="C155" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getInfo = "Naval.getInfo";</v>
+        <v>private const string CMD_enterWar = "Naval.enterWar";</v>
       </c>
       <c r="E155" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4259,14 +4272,14 @@
         <v>266</v>
       </c>
       <c r="B156" t="s">
-        <v>445</v>
+        <v>361</v>
       </c>
       <c r="C156" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getVersusCount = "Naval.getVersusCount";</v>
+        <v>private const string CMD_getInfo = "Naval.getInfo";</v>
       </c>
       <c r="E156" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4274,14 +4287,14 @@
         <v>266</v>
       </c>
       <c r="B157" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C157" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_inMissionHeros = "Naval.inMissionHeros";</v>
+        <v>private const string CMD_getVersusCount = "Naval.getVersusCount";</v>
       </c>
       <c r="E157" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4289,14 +4302,14 @@
         <v>266</v>
       </c>
       <c r="B158" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C158" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_killRank = "Naval.killRank";</v>
+        <v>private const string CMD_inMissionHeros = "Naval.inMissionHeros";</v>
       </c>
       <c r="E158" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4304,14 +4317,14 @@
         <v>266</v>
       </c>
       <c r="B159" t="s">
-        <v>323</v>
+        <v>447</v>
       </c>
       <c r="C159" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_leaveWar = "Naval.leaveWar";</v>
+        <v>private const string CMD_killRank = "Naval.killRank";</v>
       </c>
       <c r="E159" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4319,14 +4332,14 @@
         <v>266</v>
       </c>
       <c r="B160" t="s">
-        <v>448</v>
+        <v>323</v>
       </c>
       <c r="C160" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_retreatAllTroops = "Naval.retreatAllTroops";</v>
+        <v>private const string CMD_leaveWar = "Naval.leaveWar";</v>
       </c>
       <c r="E160" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4334,14 +4347,14 @@
         <v>266</v>
       </c>
       <c r="B161" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C161" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_rewardCfg = "Naval.rewardCfg";</v>
+        <v>private const string CMD_retreatAllTroops = "Naval.retreatAllTroops";</v>
       </c>
       <c r="E161" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4349,89 +4362,89 @@
         <v>266</v>
       </c>
       <c r="B162" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C162" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_sendTroops = "Naval.sendTroops";</v>
+        <v>private const string CMD_rewardCfg = "Naval.rewardCfg";</v>
       </c>
       <c r="E162" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B163" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C163" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_northCitySituation = "NorthMarch.northCitySituation";</v>
+        <v>private const string CMD_sendTroops = "Naval.sendTroops";</v>
       </c>
       <c r="E163" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B164" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C164" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_queryAllMarqueeMessage = "Notice.queryAllMarqueeMessage";</v>
+        <v>private const string CMD_northCitySituation = "NorthMarch.northCitySituation";</v>
       </c>
       <c r="E164" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B165" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C165" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getNpcWars = "NpcCorps.getNpcWars";</v>
+        <v>private const string CMD_queryAllMarqueeMessage = "Notice.queryAllMarqueeMessage";</v>
       </c>
       <c r="E165" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B166" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C166" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_cityStatus = "OneYear.cityStatus";</v>
+        <v>private const string CMD_getNpcWars = "NpcCorps.getNpcWars";</v>
       </c>
       <c r="E166" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B167" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C167" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_dealPatroledEvent = "Patrol.dealPatroledEvent";</v>
+        <v>private const string CMD_cityStatus = "OneYear.cityStatus";</v>
       </c>
       <c r="E167" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -4439,44 +4452,44 @@
         <v>271</v>
       </c>
       <c r="B168" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C168" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getPatrolInfo = "Patrol.getPatrolInfo";</v>
+        <v>private const string CMD_dealPatroledEvent = "Patrol.dealPatroledEvent";</v>
       </c>
       <c r="E168" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B169" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C169" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getPlatformInfo = "Platform.getPlatformInfo";</v>
+        <v>private const string CMD_getPatrolInfo = "Patrol.getPatrolInfo";</v>
       </c>
       <c r="E169" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B170" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C170" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getProperties = "Player.getProperties";</v>
+        <v>private const string CMD_getPlatformInfo = "Platform.getPlatformInfo";</v>
       </c>
       <c r="E170" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4484,14 +4497,14 @@
         <v>273</v>
       </c>
       <c r="B171" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C171" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getSpecialState = "Player.getSpecialState";</v>
+        <v>private const string CMD_getProperties = "Player.getProperties";</v>
       </c>
       <c r="E171" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4499,89 +4512,89 @@
         <v>273</v>
       </c>
       <c r="B172" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C172" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_updateGuideSequence = "Player.updateGuideSequence";</v>
+        <v>private const string CMD_getSpecialState = "Player.getSpecialState";</v>
       </c>
       <c r="E172" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B173" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C173" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getPrayTime = "Pray.getPrayTime";</v>
+        <v>private const string CMD_updateGuideSequence = "Player.updateGuideSequence";</v>
       </c>
       <c r="E173" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B174" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C174" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_findAllPowerRank = "Rank.findAllPowerRank";</v>
+        <v>private const string CMD_getPrayTime = "Pray.getPrayTime";</v>
       </c>
       <c r="E174" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B175" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C175" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_activityTime = "RedEnvelope.activityTime";</v>
+        <v>private const string CMD_findAllPowerRank = "Rank.findAllPowerRank";</v>
       </c>
       <c r="E175" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B176" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C176" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getSevenDayFundRewardInfo = "RewardActivity.getSevenDayFundRewardInfo";</v>
+        <v>private const string CMD_activityTime = "RedEnvelope.activityTime";</v>
       </c>
       <c r="E176" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B177" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C177" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_startRogueGangKill = "Rogue.startRogueGangKill";</v>
+        <v>private const string CMD_getSevenDayFundRewardInfo = "RewardActivity.getSevenDayFundRewardInfo";</v>
       </c>
       <c r="E177" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4589,29 +4602,29 @@
         <v>278</v>
       </c>
       <c r="B178" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C178" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_takeRogueInfo = "Rogue.takeRogueInfo";</v>
+        <v>private const string CMD_startRogueGangKill = "Rogue.startRogueGangKill";</v>
       </c>
       <c r="E178" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B179" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C179" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_availableShops = "Shop.availableShops";</v>
+        <v>private const string CMD_takeRogueInfo = "Rogue.takeRogueInfo";</v>
       </c>
       <c r="E179" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -4619,14 +4632,14 @@
         <v>279</v>
       </c>
       <c r="B180" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C180" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_buyCycleShopItem = "Shop.buyCycleShopItem";</v>
+        <v>private const string CMD_availableShops = "Shop.availableShops";</v>
       </c>
       <c r="E180" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -4634,14 +4647,14 @@
         <v>279</v>
       </c>
       <c r="B181" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C181" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_buyShopItem = "Shop.buyShopItem";</v>
+        <v>private const string CMD_buyCycleShopItem = "Shop.buyCycleShopItem";</v>
       </c>
       <c r="E181" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -4649,14 +4662,14 @@
         <v>279</v>
       </c>
       <c r="B182" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C182" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_buyTravelShopItem = "Shop.buyTravelShopItem";</v>
+        <v>private const string CMD_buyShopItem = "Shop.buyShopItem";</v>
       </c>
       <c r="E182" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -4664,14 +4677,14 @@
         <v>279</v>
       </c>
       <c r="B183" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C183" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getCycleShopInfo = "Shop.getCycleShopInfo";</v>
+        <v>private const string CMD_buyTravelShopItem = "Shop.buyTravelShopItem";</v>
       </c>
       <c r="E183" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -4679,14 +4692,14 @@
         <v>279</v>
       </c>
       <c r="B184" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C184" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getResourceTradeInfo = "Shop.getResourceTradeInfo";</v>
+        <v>private const string CMD_getCycleShopInfo = "Shop.getCycleShopInfo";</v>
       </c>
       <c r="E184" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -4694,14 +4707,14 @@
         <v>279</v>
       </c>
       <c r="B185" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C185" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getShopInfo = "Shop.getShopInfo";</v>
+        <v>private const string CMD_getResourceTradeInfo = "Shop.getResourceTradeInfo";</v>
       </c>
       <c r="E185" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4709,14 +4722,14 @@
         <v>279</v>
       </c>
       <c r="B186" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C186" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getShuangShiyiShopInfo = "Shop.getShuangShiyiShopInfo";</v>
+        <v>private const string CMD_getShopInfo = "Shop.getShopInfo";</v>
       </c>
       <c r="E186" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -4724,14 +4737,14 @@
         <v>279</v>
       </c>
       <c r="B187" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C187" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getTravelShopInfo = "Shop.getTravelShopInfo";</v>
+        <v>private const string CMD_getShuangShiyiShopInfo = "Shop.getShuangShiyiShopInfo";</v>
       </c>
       <c r="E187" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -4739,14 +4752,14 @@
         <v>279</v>
       </c>
       <c r="B188" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C188" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_otherShopsRefreshTime = "Shop.otherShopsRefreshTime";</v>
+        <v>private const string CMD_getTravelShopInfo = "Shop.getTravelShopInfo";</v>
       </c>
       <c r="E188" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -4754,14 +4767,14 @@
         <v>279</v>
       </c>
       <c r="B189" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C189" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_refreshShop = "Shop.refreshShop";</v>
+        <v>private const string CMD_otherShopsRefreshTime = "Shop.otherShopsRefreshTime";</v>
       </c>
       <c r="E189" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -4769,14 +4782,14 @@
         <v>279</v>
       </c>
       <c r="B190" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C190" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_shopNextRefreshTime = "Shop.shopNextRefreshTime";</v>
+        <v>private const string CMD_refreshShop = "Shop.refreshShop";</v>
       </c>
       <c r="E190" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -4784,29 +4797,29 @@
         <v>279</v>
       </c>
       <c r="B191" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C191" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_tradeResource = "Shop.tradeResource";</v>
+        <v>private const string CMD_shopNextRefreshTime = "Shop.shopNextRefreshTime";</v>
       </c>
       <c r="E191" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B192" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="C192" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_availableShops = "Shop2.availableShops";</v>
+        <v>private const string CMD_tradeResource = "Shop.tradeResource";</v>
       </c>
       <c r="E192" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -4814,14 +4827,14 @@
         <v>280</v>
       </c>
       <c r="B193" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="C193" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_buyItem = "Shop2.buyItem";</v>
+        <v>private const string CMD_availableShops = "Shop2.availableShops";</v>
       </c>
       <c r="E193" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -4829,29 +4842,29 @@
         <v>280</v>
       </c>
       <c r="B194" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C194" t="str">
-        <f t="shared" ref="C194:C232" si="3">CONCATENATE("private const string CMD_",B194," = """,A194,".",B194,""";")</f>
-        <v>private const string CMD_shop2Info = "Shop2.shop2Info";</v>
+        <f t="shared" si="2"/>
+        <v>private const string CMD_buyItem = "Shop2.buyItem";</v>
       </c>
       <c r="E194" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B195" t="s">
-        <v>361</v>
+        <v>481</v>
       </c>
       <c r="C195" t="str">
-        <f t="shared" si="3"/>
-        <v>private const string CMD_getInfo = "SignInReward.getInfo";</v>
+        <f t="shared" ref="C195:C233" si="3">CONCATENATE("private const string CMD_",B195," = """,A195,".",B195,""";")</f>
+        <v>private const string CMD_shop2Info = "Shop2.shop2Info";</v>
       </c>
       <c r="E195" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -4859,14 +4872,14 @@
         <v>281</v>
       </c>
       <c r="B196" t="s">
-        <v>482</v>
+        <v>361</v>
       </c>
       <c r="C196" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_signIn = "SignInReward.signIn";</v>
+        <v>private const string CMD_getInfo = "SignInReward.getInfo";</v>
       </c>
       <c r="E196" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -4874,29 +4887,29 @@
         <v>281</v>
       </c>
       <c r="B197" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C197" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_signInMultiple = "SignInReward.signInMultiple";</v>
+        <v>private const string CMD_signIn = "SignInReward.signIn";</v>
       </c>
       <c r="E197" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B198" t="s">
-        <v>379</v>
+        <v>483</v>
       </c>
       <c r="C198" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_activityInfo = "StarGazing.activityInfo";</v>
+        <v>private const string CMD_signInMultiple = "SignInReward.signInMultiple";</v>
       </c>
       <c r="E198" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -4904,44 +4917,44 @@
         <v>282</v>
       </c>
       <c r="B199" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C199" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_myFirecrackerInfo = "StarGazing.myFirecrackerInfo";</v>
+        <v>private const string CMD_activityInfo = "StarGazing.activityInfo";</v>
       </c>
       <c r="E199" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B200" t="s">
-        <v>484</v>
+        <v>380</v>
       </c>
       <c r="C200" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_ping = "System.ping";</v>
+        <v>private const string CMD_myFirecrackerInfo = "StarGazing.myFirecrackerInfo";</v>
       </c>
       <c r="E200" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B201" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C201" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_finishTask = "Task.finishTask";</v>
+        <v>private const string CMD_ping = "System.ping";</v>
       </c>
       <c r="E201" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -4949,14 +4962,14 @@
         <v>284</v>
       </c>
       <c r="B202" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C202" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getAchievementInfo = "Task.getAchievementInfo";</v>
+        <v>private const string CMD_finishTask = "Task.finishTask";</v>
       </c>
       <c r="E202" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -4964,44 +4977,44 @@
         <v>284</v>
       </c>
       <c r="B203" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C203" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getTaskTraceInfo = "Task.getTaskTraceInfo";</v>
+        <v>private const string CMD_getAchievementInfo = "Task.getAchievementInfo";</v>
       </c>
       <c r="E203" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B204" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C204" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_teamDuplicateFreeTimes = "TeamDuplicate.teamDuplicateFreeTimes";</v>
+        <v>private const string CMD_getTaskTraceInfo = "Task.getTaskTraceInfo";</v>
       </c>
       <c r="E204" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B205" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C205" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_arriveStep = "Travel.arriveStep";</v>
+        <v>private const string CMD_teamDuplicateFreeTimes = "TeamDuplicate.teamDuplicateFreeTimes";</v>
       </c>
       <c r="E205" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -5009,14 +5022,14 @@
         <v>286</v>
       </c>
       <c r="B206" t="s">
-        <v>367</v>
+        <v>489</v>
       </c>
       <c r="C206" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_attack = "Travel.attack";</v>
+        <v>private const string CMD_arriveStep = "Travel.arriveStep";</v>
       </c>
       <c r="E206" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -5024,14 +5037,14 @@
         <v>286</v>
       </c>
       <c r="B207" t="s">
-        <v>490</v>
+        <v>367</v>
       </c>
       <c r="C207" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_checkOut = "Travel.checkOut";</v>
+        <v>private const string CMD_attack = "Travel.attack";</v>
       </c>
       <c r="E207" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5039,14 +5052,14 @@
         <v>286</v>
       </c>
       <c r="B208" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C208" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_controlDice = "Travel.controlDice";</v>
+        <v>private const string CMD_checkOut = "Travel.checkOut";</v>
       </c>
       <c r="E208" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5054,14 +5067,14 @@
         <v>286</v>
       </c>
       <c r="B209" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C209" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_dice = "Travel.dice";</v>
+        <v>private const string CMD_controlDice = "Travel.controlDice";</v>
       </c>
       <c r="E209" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5069,14 +5082,14 @@
         <v>286</v>
       </c>
       <c r="B210" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C210" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_escape = "Travel.escape";</v>
+        <v>private const string CMD_dice = "Travel.dice";</v>
       </c>
       <c r="E210" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -5084,14 +5097,14 @@
         <v>286</v>
       </c>
       <c r="B211" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C211" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getMapInfo = "Travel.getMapInfo";</v>
+        <v>private const string CMD_escape = "Travel.escape";</v>
       </c>
       <c r="E211" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -5099,14 +5112,14 @@
         <v>286</v>
       </c>
       <c r="B212" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C212" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getStatus = "Travel.getStatus";</v>
+        <v>private const string CMD_getMapInfo = "Travel.getMapInfo";</v>
       </c>
       <c r="E212" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -5114,14 +5127,14 @@
         <v>286</v>
       </c>
       <c r="B213" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C213" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_restartTravel = "Travel.restartTravel";</v>
+        <v>private const string CMD_getStatus = "Travel.getStatus";</v>
       </c>
       <c r="E213" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5129,29 +5142,29 @@
         <v>286</v>
       </c>
       <c r="B214" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C214" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_viewStep = "Travel.viewStep";</v>
+        <v>private const string CMD_restartTravel = "Travel.restartTravel";</v>
       </c>
       <c r="E214" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B215" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C215" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getTurnCardRewards = "TurnCardReward.getTurnCardRewards";</v>
+        <v>private const string CMD_viewStep = "Travel.viewStep";</v>
       </c>
       <c r="E215" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -5159,44 +5172,44 @@
         <v>287</v>
       </c>
       <c r="B216" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C216" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_turnCard = "TurnCardReward.turnCard";</v>
+        <v>private const string CMD_getTurnCardRewards = "TurnCardReward.getTurnCardRewards";</v>
       </c>
       <c r="E216" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B217" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C217" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getActivityInfo = "Valentine.getActivityInfo";</v>
+        <v>private const string CMD_turnCard = "TurnCardReward.turnCard";</v>
       </c>
       <c r="E217" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B218" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C218" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_firstChargeInfo = "Vip.firstChargeInfo";</v>
+        <v>private const string CMD_getActivityInfo = "Valentine.getActivityInfo";</v>
       </c>
       <c r="E218" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5204,14 +5217,14 @@
         <v>289</v>
       </c>
       <c r="B219" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C219" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_monthCard = "Vip.monthCard";</v>
+        <v>private const string CMD_firstChargeInfo = "Vip.firstChargeInfo";</v>
       </c>
       <c r="E219" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -5219,59 +5232,59 @@
         <v>289</v>
       </c>
       <c r="B220" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C220" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_vipPrivilegeLevel = "Vip.vipPrivilegeLevel";</v>
+        <v>private const string CMD_monthCard = "Vip.monthCard";</v>
       </c>
       <c r="E220" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B221" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C221" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_isGotMobileGift = "VipAuthentication.isGotMobileGift";</v>
+        <v>private const string CMD_vipPrivilegeLevel = "Vip.vipPrivilegeLevel";</v>
       </c>
       <c r="E221" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B222" t="s">
-        <v>341</v>
+        <v>504</v>
       </c>
       <c r="C222" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_time = "WelfareLottery.time";</v>
+        <v>private const string CMD_isGotMobileGift = "VipAuthentication.isGotMobileGift";</v>
       </c>
       <c r="E222" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B223" t="s">
-        <v>505</v>
+        <v>341</v>
       </c>
       <c r="C223" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_citySituationDetail = "World.citySituationDetail";</v>
+        <v>private const string CMD_time = "WelfareLottery.time";</v>
       </c>
       <c r="E223" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5279,14 +5292,14 @@
         <v>292</v>
       </c>
       <c r="B224" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C224" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getAllOpenedCities = "World.getAllOpenedCities";</v>
+        <v>private const string CMD_citySituationDetail = "World.citySituationDetail";</v>
       </c>
       <c r="E224" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -5294,14 +5307,14 @@
         <v>292</v>
       </c>
       <c r="B225" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C225" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getAllTransportingUnits = "World.getAllTransportingUnits";</v>
+        <v>private const string CMD_getAllOpenedCities = "World.getAllOpenedCities";</v>
       </c>
       <c r="E225" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -5309,14 +5322,14 @@
         <v>292</v>
       </c>
       <c r="B226" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C226" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getCityChapterBlueprint = "World.getCityChapterBlueprint";</v>
+        <v>private const string CMD_getAllTransportingUnits = "World.getAllTransportingUnits";</v>
       </c>
       <c r="E226" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -5324,14 +5337,14 @@
         <v>292</v>
       </c>
       <c r="B227" t="s">
-        <v>351</v>
+        <v>508</v>
       </c>
       <c r="C227" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getCityRewardInfo = "World.getCityRewardInfo";</v>
+        <v>private const string CMD_getCityChapterBlueprint = "World.getCityChapterBlueprint";</v>
       </c>
       <c r="E227" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -5339,14 +5352,14 @@
         <v>292</v>
       </c>
       <c r="B228" t="s">
-        <v>509</v>
+        <v>351</v>
       </c>
       <c r="C228" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getExploredWorldArea = "World.getExploredWorldArea";</v>
+        <v>private const string CMD_getCityRewardInfo = "World.getCityRewardInfo";</v>
       </c>
       <c r="E228" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -5354,14 +5367,14 @@
         <v>292</v>
       </c>
       <c r="B229" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C229" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_go = "World.go";</v>
+        <v>private const string CMD_getExploredWorldArea = "World.getExploredWorldArea";</v>
       </c>
       <c r="E229" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -5369,43 +5382,58 @@
         <v>292</v>
       </c>
       <c r="B230" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C230" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_worldSituation = "World.worldSituation";</v>
+        <v>private const string CMD_go = "World.go";</v>
       </c>
       <c r="E230" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B231" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C231" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getYunYouInfo = "YunYou.getYunYouInfo";</v>
+        <v>private const string CMD_worldSituation = "World.worldSituation";</v>
       </c>
       <c r="E231" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B232" t="s">
-        <v>318</v>
+        <v>512</v>
       </c>
       <c r="C232" t="str">
         <f t="shared" si="3"/>
+        <v>private const string CMD_getYunYouInfo = "YunYou.getYunYouInfo";</v>
+      </c>
+      <c r="E232" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>294</v>
+      </c>
+      <c r="B233" t="s">
+        <v>318</v>
+      </c>
+      <c r="C233" t="str">
+        <f t="shared" si="3"/>
         <v>private const string CMD_getTimeInfo = "ZaJinDan.getTimeInfo";</v>
       </c>
-      <c r="E232" t="s">
+      <c r="E233" t="s">
         <v>231</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New packet for 北伐匈奴
</commit_message>
<xml_diff>
--- a/PacketInfo/Sample.xlsx
+++ b/PacketInfo/Sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="520">
   <si>
     <t xml:space="preserve"> {"act":"Activity.drawCompanyAnniversaryLoginReward","sid":"3fc3b84cbd46610e7363daf513b792a962898752"}</t>
   </si>
@@ -1569,6 +1569,21 @@
   </si>
   <si>
     <t>{"act":"Activity.getShuangShiyiActivityReward","sid":"3fc3b84cbd46610e7363daf533d182bd500440a7"}</t>
+  </si>
+  <si>
+    <t>{"act":"NorthMarch.enterWar","sid":"3fc3b84cbd46610e7363daf533d182bd500440a7"}</t>
+  </si>
+  <si>
+    <t>{"act":"NorthMarch.retreatAllTroops","sid":"3fc3b84cbd46610e7363daf533d182bd500440a7"}</t>
+  </si>
+  <si>
+    <t>{"act":"NorthMarch.inMissionHeros","sid":"3fc3b84cbd46610e7363daf533d182bd500440a7"}</t>
+  </si>
+  <si>
+    <t>{"act":"NorthMarch.sendTroops","sid":"3fc3b84cbd46610e7363daf533d182bd500440a7","body":"{\"cityId\":129,\"save\":{\"chief\":28,\"heros\":[{\"x\":-2,\"y\":0,\"index\":42},{\"x\":-3,\"y\":-1,\"index\":28},{\"x\":-5,\"y\":-1,\"index\":17},{\"x\":-3,\"y\":1,\"index\":15},{\"x\":-5,\"y\":1,\"index\":9}]},\"type\":\"NORTH_WAR\"}"}</t>
+  </si>
+  <si>
+    <t>{"act":"NorthMarch.leaveWar","sid":"3fc3b84cbd46610e7363daf533d182bd500440a7"}</t>
   </si>
 </sst>
 </file>
@@ -1927,10 +1942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:E238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="B145" workbookViewId="0">
+      <selection activeCell="C164" sqref="C164:C169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3900,7 +3915,7 @@
         <v>421</v>
       </c>
       <c r="C131" t="str">
-        <f t="shared" ref="C131:C194" si="2">CONCATENATE("private const string CMD_",B131," = """,A131,".",B131,""";")</f>
+        <f t="shared" ref="C131:C199" si="2">CONCATENATE("private const string CMD_",B131," = """,A131,".",B131,""";")</f>
         <v>private const string CMD_appointHero = "Manor.appointHero";</v>
       </c>
       <c r="E131" t="s">
@@ -4387,319 +4402,319 @@
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+    <row r="164" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B164" t="s">
-        <v>451</v>
-      </c>
-      <c r="C164" t="str">
-        <f t="shared" si="2"/>
-        <v>private const string CMD_northCitySituation = "NorthMarch.northCitySituation";</v>
-      </c>
-      <c r="E164" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>268</v>
-      </c>
-      <c r="B165" t="s">
-        <v>452</v>
-      </c>
-      <c r="C165" t="str">
-        <f t="shared" si="2"/>
-        <v>private const string CMD_queryAllMarqueeMessage = "Notice.queryAllMarqueeMessage";</v>
-      </c>
-      <c r="E165" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>269</v>
-      </c>
-      <c r="B166" t="s">
-        <v>453</v>
-      </c>
-      <c r="C166" t="str">
-        <f t="shared" si="2"/>
-        <v>private const string CMD_getNpcWars = "NpcCorps.getNpcWars";</v>
-      </c>
-      <c r="E166" t="s">
-        <v>164</v>
+      <c r="B164" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C164" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>private const string CMD_enterWar = "NorthMarch.enterWar";</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C165" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>private const string CMD_inMissionHeros = "NorthMarch.inMissionHeros";</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C166" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>private const string CMD_leaveWar = "NorthMarch.leaveWar";</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B167" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C167" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_cityStatus = "OneYear.cityStatus";</v>
+        <v>private const string CMD_northCitySituation = "NorthMarch.northCitySituation";</v>
       </c>
       <c r="E167" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>271</v>
-      </c>
-      <c r="B168" t="s">
-        <v>455</v>
-      </c>
-      <c r="C168" t="str">
-        <f t="shared" si="2"/>
-        <v>private const string CMD_dealPatroledEvent = "Patrol.dealPatroledEvent";</v>
-      </c>
-      <c r="E168" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>271</v>
-      </c>
-      <c r="B169" t="s">
-        <v>456</v>
-      </c>
-      <c r="C169" t="str">
-        <f t="shared" si="2"/>
-        <v>private const string CMD_getPatrolInfo = "Patrol.getPatrolInfo";</v>
-      </c>
-      <c r="E169" t="s">
-        <v>167</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C168" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>private const string CMD_retreatAllTroops = "NorthMarch.retreatAllTroops";</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C169" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>private const string CMD_sendTroops = "NorthMarch.sendTroops";</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B170" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="C170" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getPlatformInfo = "Platform.getPlatformInfo";</v>
+        <v>private const string CMD_queryAllMarqueeMessage = "Notice.queryAllMarqueeMessage";</v>
       </c>
       <c r="E170" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B171" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C171" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getProperties = "Player.getProperties";</v>
+        <v>private const string CMD_getNpcWars = "NpcCorps.getNpcWars";</v>
       </c>
       <c r="E171" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B172" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="C172" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getSpecialState = "Player.getSpecialState";</v>
+        <v>private const string CMD_cityStatus = "OneYear.cityStatus";</v>
       </c>
       <c r="E172" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B173" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="C173" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_updateGuideSequence = "Player.updateGuideSequence";</v>
+        <v>private const string CMD_dealPatroledEvent = "Patrol.dealPatroledEvent";</v>
       </c>
       <c r="E173" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B174" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="C174" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getPrayTime = "Pray.getPrayTime";</v>
+        <v>private const string CMD_getPatrolInfo = "Patrol.getPatrolInfo";</v>
       </c>
       <c r="E174" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B175" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="C175" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_findAllPowerRank = "Rank.findAllPowerRank";</v>
+        <v>private const string CMD_getPlatformInfo = "Platform.getPlatformInfo";</v>
       </c>
       <c r="E175" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B176" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="C176" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_activityTime = "RedEnvelope.activityTime";</v>
+        <v>private const string CMD_getProperties = "Player.getProperties";</v>
       </c>
       <c r="E176" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B177" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C177" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getSevenDayFundRewardInfo = "RewardActivity.getSevenDayFundRewardInfo";</v>
+        <v>private const string CMD_getSpecialState = "Player.getSpecialState";</v>
       </c>
       <c r="E177" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B178" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C178" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_startRogueGangKill = "Rogue.startRogueGangKill";</v>
+        <v>private const string CMD_updateGuideSequence = "Player.updateGuideSequence";</v>
       </c>
       <c r="E178" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B179" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="C179" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_takeRogueInfo = "Rogue.takeRogueInfo";</v>
+        <v>private const string CMD_getPrayTime = "Pray.getPrayTime";</v>
       </c>
       <c r="E179" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B180" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C180" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_availableShops = "Shop.availableShops";</v>
+        <v>private const string CMD_findAllPowerRank = "Rank.findAllPowerRank";</v>
       </c>
       <c r="E180" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B181" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C181" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_buyCycleShopItem = "Shop.buyCycleShopItem";</v>
+        <v>private const string CMD_activityTime = "RedEnvelope.activityTime";</v>
       </c>
       <c r="E181" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B182" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="C182" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_buyShopItem = "Shop.buyShopItem";</v>
+        <v>private const string CMD_getSevenDayFundRewardInfo = "RewardActivity.getSevenDayFundRewardInfo";</v>
       </c>
       <c r="E182" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B183" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="C183" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_buyTravelShopItem = "Shop.buyTravelShopItem";</v>
+        <v>private const string CMD_startRogueGangKill = "Rogue.startRogueGangKill";</v>
       </c>
       <c r="E183" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B184" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="C184" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getCycleShopInfo = "Shop.getCycleShopInfo";</v>
+        <v>private const string CMD_takeRogueInfo = "Rogue.takeRogueInfo";</v>
       </c>
       <c r="E184" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -4707,14 +4722,14 @@
         <v>279</v>
       </c>
       <c r="B185" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="C185" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getResourceTradeInfo = "Shop.getResourceTradeInfo";</v>
+        <v>private const string CMD_availableShops = "Shop.availableShops";</v>
       </c>
       <c r="E185" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4722,14 +4737,14 @@
         <v>279</v>
       </c>
       <c r="B186" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C186" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getShopInfo = "Shop.getShopInfo";</v>
+        <v>private const string CMD_buyCycleShopItem = "Shop.buyCycleShopItem";</v>
       </c>
       <c r="E186" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -4737,14 +4752,14 @@
         <v>279</v>
       </c>
       <c r="B187" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C187" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getShuangShiyiShopInfo = "Shop.getShuangShiyiShopInfo";</v>
+        <v>private const string CMD_buyShopItem = "Shop.buyShopItem";</v>
       </c>
       <c r="E187" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -4752,14 +4767,14 @@
         <v>279</v>
       </c>
       <c r="B188" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="C188" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_getTravelShopInfo = "Shop.getTravelShopInfo";</v>
+        <v>private const string CMD_buyTravelShopItem = "Shop.buyTravelShopItem";</v>
       </c>
       <c r="E188" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -4767,14 +4782,14 @@
         <v>279</v>
       </c>
       <c r="B189" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="C189" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_otherShopsRefreshTime = "Shop.otherShopsRefreshTime";</v>
+        <v>private const string CMD_getCycleShopInfo = "Shop.getCycleShopInfo";</v>
       </c>
       <c r="E189" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -4782,14 +4797,14 @@
         <v>279</v>
       </c>
       <c r="B190" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C190" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_refreshShop = "Shop.refreshShop";</v>
+        <v>private const string CMD_getResourceTradeInfo = "Shop.getResourceTradeInfo";</v>
       </c>
       <c r="E190" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -4797,14 +4812,14 @@
         <v>279</v>
       </c>
       <c r="B191" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C191" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_shopNextRefreshTime = "Shop.shopNextRefreshTime";</v>
+        <v>private const string CMD_getShopInfo = "Shop.getShopInfo";</v>
       </c>
       <c r="E191" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -4812,284 +4827,284 @@
         <v>279</v>
       </c>
       <c r="B192" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C192" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_tradeResource = "Shop.tradeResource";</v>
+        <v>private const string CMD_getShuangShiyiShopInfo = "Shop.getShuangShiyiShopInfo";</v>
       </c>
       <c r="E192" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B193" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="C193" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_availableShops = "Shop2.availableShops";</v>
+        <v>private const string CMD_getTravelShopInfo = "Shop.getTravelShopInfo";</v>
       </c>
       <c r="E193" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B194" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C194" t="str">
         <f t="shared" si="2"/>
-        <v>private const string CMD_buyItem = "Shop2.buyItem";</v>
+        <v>private const string CMD_otherShopsRefreshTime = "Shop.otherShopsRefreshTime";</v>
       </c>
       <c r="E194" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B195" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C195" t="str">
-        <f t="shared" ref="C195:C233" si="3">CONCATENATE("private const string CMD_",B195," = """,A195,".",B195,""";")</f>
-        <v>private const string CMD_shop2Info = "Shop2.shop2Info";</v>
+        <f t="shared" si="2"/>
+        <v>private const string CMD_refreshShop = "Shop.refreshShop";</v>
       </c>
       <c r="E195" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
+        <v>279</v>
+      </c>
+      <c r="B196" t="s">
+        <v>478</v>
+      </c>
+      <c r="C196" t="str">
+        <f t="shared" si="2"/>
+        <v>private const string CMD_shopNextRefreshTime = "Shop.shopNextRefreshTime";</v>
+      </c>
+      <c r="E196" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>279</v>
+      </c>
+      <c r="B197" t="s">
+        <v>479</v>
+      </c>
+      <c r="C197" t="str">
+        <f t="shared" si="2"/>
+        <v>private const string CMD_tradeResource = "Shop.tradeResource";</v>
+      </c>
+      <c r="E197" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>280</v>
+      </c>
+      <c r="B198" t="s">
+        <v>467</v>
+      </c>
+      <c r="C198" t="str">
+        <f t="shared" si="2"/>
+        <v>private const string CMD_availableShops = "Shop2.availableShops";</v>
+      </c>
+      <c r="E198" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>280</v>
+      </c>
+      <c r="B199" t="s">
+        <v>480</v>
+      </c>
+      <c r="C199" t="str">
+        <f t="shared" si="2"/>
+        <v>private const string CMD_buyItem = "Shop2.buyItem";</v>
+      </c>
+      <c r="E199" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>280</v>
+      </c>
+      <c r="B200" t="s">
+        <v>481</v>
+      </c>
+      <c r="C200" t="str">
+        <f t="shared" ref="C200:C238" si="3">CONCATENATE("private const string CMD_",B200," = """,A200,".",B200,""";")</f>
+        <v>private const string CMD_shop2Info = "Shop2.shop2Info";</v>
+      </c>
+      <c r="E200" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>281</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B201" t="s">
         <v>361</v>
       </c>
-      <c r="C196" t="str">
+      <c r="C201" t="str">
         <f t="shared" si="3"/>
         <v>private const string CMD_getInfo = "SignInReward.getInfo";</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E201" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>281</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B202" t="s">
         <v>482</v>
       </c>
-      <c r="C197" t="str">
+      <c r="C202" t="str">
         <f t="shared" si="3"/>
         <v>private const string CMD_signIn = "SignInReward.signIn";</v>
       </c>
-      <c r="E197" t="s">
+      <c r="E202" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
         <v>281</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B203" t="s">
         <v>483</v>
       </c>
-      <c r="C198" t="str">
+      <c r="C203" t="str">
         <f t="shared" si="3"/>
         <v>private const string CMD_signInMultiple = "SignInReward.signInMultiple";</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E203" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>282</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B204" t="s">
         <v>379</v>
       </c>
-      <c r="C199" t="str">
+      <c r="C204" t="str">
         <f t="shared" si="3"/>
         <v>private const string CMD_activityInfo = "StarGazing.activityInfo";</v>
       </c>
-      <c r="E199" t="s">
+      <c r="E204" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>282</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B205" t="s">
         <v>380</v>
       </c>
-      <c r="C200" t="str">
+      <c r="C205" t="str">
         <f t="shared" si="3"/>
         <v>private const string CMD_myFirecrackerInfo = "StarGazing.myFirecrackerInfo";</v>
       </c>
-      <c r="E200" t="s">
+      <c r="E205" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>283</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B206" t="s">
         <v>484</v>
       </c>
-      <c r="C201" t="str">
+      <c r="C206" t="str">
         <f t="shared" si="3"/>
         <v>private const string CMD_ping = "System.ping";</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E206" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>284</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B207" t="s">
         <v>485</v>
       </c>
-      <c r="C202" t="str">
+      <c r="C207" t="str">
         <f t="shared" si="3"/>
         <v>private const string CMD_finishTask = "Task.finishTask";</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E207" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>284</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B208" t="s">
         <v>486</v>
       </c>
-      <c r="C203" t="str">
+      <c r="C208" t="str">
         <f t="shared" si="3"/>
         <v>private const string CMD_getAchievementInfo = "Task.getAchievementInfo";</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E208" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>284</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B209" t="s">
         <v>487</v>
       </c>
-      <c r="C204" t="str">
+      <c r="C209" t="str">
         <f t="shared" si="3"/>
         <v>private const string CMD_getTaskTraceInfo = "Task.getTaskTraceInfo";</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E209" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
         <v>285</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B210" t="s">
         <v>488</v>
       </c>
-      <c r="C205" t="str">
+      <c r="C210" t="str">
         <f t="shared" si="3"/>
         <v>private const string CMD_teamDuplicateFreeTimes = "TeamDuplicate.teamDuplicateFreeTimes";</v>
       </c>
-      <c r="E205" t="s">
+      <c r="E210" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>286</v>
-      </c>
-      <c r="B206" t="s">
-        <v>489</v>
-      </c>
-      <c r="C206" t="str">
-        <f t="shared" si="3"/>
-        <v>private const string CMD_arriveStep = "Travel.arriveStep";</v>
-      </c>
-      <c r="E206" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>286</v>
-      </c>
-      <c r="B207" t="s">
-        <v>367</v>
-      </c>
-      <c r="C207" t="str">
-        <f t="shared" si="3"/>
-        <v>private const string CMD_attack = "Travel.attack";</v>
-      </c>
-      <c r="E207" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>286</v>
-      </c>
-      <c r="B208" t="s">
-        <v>490</v>
-      </c>
-      <c r="C208" t="str">
-        <f t="shared" si="3"/>
-        <v>private const string CMD_checkOut = "Travel.checkOut";</v>
-      </c>
-      <c r="E208" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>286</v>
-      </c>
-      <c r="B209" t="s">
-        <v>491</v>
-      </c>
-      <c r="C209" t="str">
-        <f t="shared" si="3"/>
-        <v>private const string CMD_controlDice = "Travel.controlDice";</v>
-      </c>
-      <c r="E209" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>286</v>
-      </c>
-      <c r="B210" t="s">
-        <v>492</v>
-      </c>
-      <c r="C210" t="str">
-        <f t="shared" si="3"/>
-        <v>private const string CMD_dice = "Travel.dice";</v>
-      </c>
-      <c r="E210" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -5097,14 +5112,14 @@
         <v>286</v>
       </c>
       <c r="B211" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C211" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_escape = "Travel.escape";</v>
+        <v>private const string CMD_arriveStep = "Travel.arriveStep";</v>
       </c>
       <c r="E211" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -5112,14 +5127,14 @@
         <v>286</v>
       </c>
       <c r="B212" t="s">
-        <v>494</v>
+        <v>367</v>
       </c>
       <c r="C212" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getMapInfo = "Travel.getMapInfo";</v>
+        <v>private const string CMD_attack = "Travel.attack";</v>
       </c>
       <c r="E212" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -5127,14 +5142,14 @@
         <v>286</v>
       </c>
       <c r="B213" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="C213" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getStatus = "Travel.getStatus";</v>
+        <v>private const string CMD_checkOut = "Travel.checkOut";</v>
       </c>
       <c r="E213" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5142,14 +5157,14 @@
         <v>286</v>
       </c>
       <c r="B214" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="C214" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_restartTravel = "Travel.restartTravel";</v>
+        <v>private const string CMD_controlDice = "Travel.controlDice";</v>
       </c>
       <c r="E214" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5157,209 +5172,209 @@
         <v>286</v>
       </c>
       <c r="B215" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="C215" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_viewStep = "Travel.viewStep";</v>
+        <v>private const string CMD_dice = "Travel.dice";</v>
       </c>
       <c r="E215" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B216" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="C216" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getTurnCardRewards = "TurnCardReward.getTurnCardRewards";</v>
+        <v>private const string CMD_escape = "Travel.escape";</v>
       </c>
       <c r="E216" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B217" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="C217" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_turnCard = "TurnCardReward.turnCard";</v>
+        <v>private const string CMD_getMapInfo = "Travel.getMapInfo";</v>
       </c>
       <c r="E217" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B218" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C218" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getActivityInfo = "Valentine.getActivityInfo";</v>
+        <v>private const string CMD_getStatus = "Travel.getStatus";</v>
       </c>
       <c r="E218" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B219" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="C219" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_firstChargeInfo = "Vip.firstChargeInfo";</v>
+        <v>private const string CMD_restartTravel = "Travel.restartTravel";</v>
       </c>
       <c r="E219" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B220" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="C220" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_monthCard = "Vip.monthCard";</v>
+        <v>private const string CMD_viewStep = "Travel.viewStep";</v>
       </c>
       <c r="E220" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B221" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="C221" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_vipPrivilegeLevel = "Vip.vipPrivilegeLevel";</v>
+        <v>private const string CMD_getTurnCardRewards = "TurnCardReward.getTurnCardRewards";</v>
       </c>
       <c r="E221" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B222" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C222" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_isGotMobileGift = "VipAuthentication.isGotMobileGift";</v>
+        <v>private const string CMD_turnCard = "TurnCardReward.turnCard";</v>
       </c>
       <c r="E222" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B223" t="s">
-        <v>341</v>
+        <v>500</v>
       </c>
       <c r="C223" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_time = "WelfareLottery.time";</v>
+        <v>private const string CMD_getActivityInfo = "Valentine.getActivityInfo";</v>
       </c>
       <c r="E223" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B224" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C224" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_citySituationDetail = "World.citySituationDetail";</v>
+        <v>private const string CMD_firstChargeInfo = "Vip.firstChargeInfo";</v>
       </c>
       <c r="E224" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B225" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C225" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getAllOpenedCities = "World.getAllOpenedCities";</v>
+        <v>private const string CMD_monthCard = "Vip.monthCard";</v>
       </c>
       <c r="E225" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B226" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C226" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getAllTransportingUnits = "World.getAllTransportingUnits";</v>
+        <v>private const string CMD_vipPrivilegeLevel = "Vip.vipPrivilegeLevel";</v>
       </c>
       <c r="E226" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B227" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C227" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getCityChapterBlueprint = "World.getCityChapterBlueprint";</v>
+        <v>private const string CMD_isGotMobileGift = "VipAuthentication.isGotMobileGift";</v>
       </c>
       <c r="E227" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B228" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="C228" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getCityRewardInfo = "World.getCityRewardInfo";</v>
+        <v>private const string CMD_time = "WelfareLottery.time";</v>
       </c>
       <c r="E228" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -5367,14 +5382,14 @@
         <v>292</v>
       </c>
       <c r="B229" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C229" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getExploredWorldArea = "World.getExploredWorldArea";</v>
+        <v>private const string CMD_citySituationDetail = "World.citySituationDetail";</v>
       </c>
       <c r="E229" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -5382,14 +5397,14 @@
         <v>292</v>
       </c>
       <c r="B230" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C230" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_go = "World.go";</v>
+        <v>private const string CMD_getAllOpenedCities = "World.getAllOpenedCities";</v>
       </c>
       <c r="E230" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -5397,43 +5412,118 @@
         <v>292</v>
       </c>
       <c r="B231" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C231" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_worldSituation = "World.worldSituation";</v>
+        <v>private const string CMD_getAllTransportingUnits = "World.getAllTransportingUnits";</v>
       </c>
       <c r="E231" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B232" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C232" t="str">
         <f t="shared" si="3"/>
-        <v>private const string CMD_getYunYouInfo = "YunYou.getYunYouInfo";</v>
+        <v>private const string CMD_getCityChapterBlueprint = "World.getCityChapterBlueprint";</v>
       </c>
       <c r="E232" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B233" t="s">
-        <v>318</v>
+        <v>351</v>
       </c>
       <c r="C233" t="str">
         <f t="shared" si="3"/>
+        <v>private const string CMD_getCityRewardInfo = "World.getCityRewardInfo";</v>
+      </c>
+      <c r="E233" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>292</v>
+      </c>
+      <c r="B234" t="s">
+        <v>509</v>
+      </c>
+      <c r="C234" t="str">
+        <f t="shared" si="3"/>
+        <v>private const string CMD_getExploredWorldArea = "World.getExploredWorldArea";</v>
+      </c>
+      <c r="E234" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>292</v>
+      </c>
+      <c r="B235" t="s">
+        <v>510</v>
+      </c>
+      <c r="C235" t="str">
+        <f t="shared" si="3"/>
+        <v>private const string CMD_go = "World.go";</v>
+      </c>
+      <c r="E235" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>292</v>
+      </c>
+      <c r="B236" t="s">
+        <v>511</v>
+      </c>
+      <c r="C236" t="str">
+        <f t="shared" si="3"/>
+        <v>private const string CMD_worldSituation = "World.worldSituation";</v>
+      </c>
+      <c r="E236" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>293</v>
+      </c>
+      <c r="B237" t="s">
+        <v>512</v>
+      </c>
+      <c r="C237" t="str">
+        <f t="shared" si="3"/>
+        <v>private const string CMD_getYunYouInfo = "YunYou.getYunYouInfo";</v>
+      </c>
+      <c r="E237" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>294</v>
+      </c>
+      <c r="B238" t="s">
+        <v>318</v>
+      </c>
+      <c r="C238" t="str">
+        <f t="shared" si="3"/>
         <v>private const string CMD_getTimeInfo = "ZaJinDan.getTimeInfo";</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E238" t="s">
         <v>231</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Just to commit the saved XLSX
</commit_message>
<xml_diff>
--- a/PacketInfo/Sample.xlsx
+++ b/PacketInfo/Sample.xlsx
@@ -1667,18 +1667,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1694,13 +1688,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2020,9 +2012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G248"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E207" sqref="E207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,7 +2025,7 @@
     <col min="4" max="4" width="43.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="247.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.125" style="1"/>
-    <col min="7" max="7" width="190.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="190.625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
@@ -2055,7 +2047,7 @@
         <f>IFERROR(FIND("body",E1),-1)</f>
         <v>-1</v>
       </c>
-      <c r="G1" s="3" t="str">
+      <c r="G1" s="1" t="str">
         <f>IF(F1&lt;0,CONCATENATE("public static RequestReturnObject ",B1,"(HTTPRequestHeaders oH, string sid)",CHAR(13),"{",CHAR(13),"return com.SendGenericRequest(oH, sid, CMD_",B1,");",CHAR(13),"}",CHAR(13)),"")</f>
         <v>public static RequestReturnObject drawCompanyAnniversaryLoginReward(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_drawCompanyAnniversaryLoginReward);_x000D_}_x000D_</v>
       </c>
@@ -2078,7 +2070,7 @@
         <f t="shared" ref="F2:F75" si="1">IFERROR(FIND("body",E2),-1)</f>
         <v>-1</v>
       </c>
-      <c r="G2" s="3" t="str">
+      <c r="G2" s="1" t="str">
         <f t="shared" ref="G2:G75" si="2">IF(F2&lt;0,CONCATENATE("public static RequestReturnObject ",B2,"(HTTPRequestHeaders oH, string sid)",CHAR(13),"{",CHAR(13),"return com.SendGenericRequest(oH, sid, CMD_",B2,");",CHAR(13),"}",CHAR(13)),"")</f>
         <v>public static RequestReturnObject drawCompanyAnniversaryRechargeReward(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_drawCompanyAnniversaryRechargeReward);_x000D_}_x000D_</v>
       </c>
@@ -2101,7 +2093,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G3" s="3" t="str">
+      <c r="G3" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject drawExchangeHoliday(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_drawExchangeHoliday);_x000D_}_x000D_</v>
       </c>
@@ -2124,7 +2116,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G4" s="3" t="str">
+      <c r="G4" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject drawStrategicFundInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_drawStrategicFundInfo);_x000D_}_x000D_</v>
       </c>
@@ -2147,7 +2139,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G5" s="3" t="str">
+      <c r="G5" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getActivityList(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getActivityList);_x000D_}_x000D_</v>
       </c>
@@ -2170,7 +2162,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G6" s="3" t="str">
+      <c r="G6" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getAnnouncement(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getAnnouncement);_x000D_}_x000D_</v>
       </c>
@@ -2193,7 +2185,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G7" s="3" t="str">
+      <c r="G7" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getBookHeroInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getBookHeroInfo);_x000D_}_x000D_</v>
       </c>
@@ -2216,7 +2208,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G8" s="3" t="str">
+      <c r="G8" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getCloudSellerInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getCloudSellerInfo);_x000D_}_x000D_</v>
       </c>
@@ -2239,7 +2231,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G9" s="3" t="str">
+      <c r="G9" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getPlayerGoBackActivityInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getPlayerGoBackActivityInfo);_x000D_}_x000D_</v>
       </c>
@@ -2262,7 +2254,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G10" s="3" t="str">
+      <c r="G10" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getRankInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getRankInfo);_x000D_}_x000D_</v>
       </c>
@@ -2285,7 +2277,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G11" s="3" t="str">
+      <c r="G11" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getRationActivity(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getRationActivity);_x000D_}_x000D_</v>
       </c>
@@ -2308,7 +2300,7 @@
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="G12" s="3" t="str">
+      <c r="G12" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2331,7 +2323,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G13" s="3" t="str">
+      <c r="G13" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getShuangShiyiActivityInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getShuangShiyiActivityInfo);_x000D_}_x000D_</v>
       </c>
@@ -2354,7 +2346,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G14" s="3" t="str">
+      <c r="G14" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getShuangShiyiActivityReward(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getShuangShiyiActivityReward);_x000D_}_x000D_</v>
       </c>
@@ -2377,7 +2369,7 @@
         <f t="shared" ref="F15" si="3">IFERROR(FIND("body",E15),-1)</f>
         <v>-1</v>
       </c>
-      <c r="G15" s="3" t="str">
+      <c r="G15" s="1" t="str">
         <f t="shared" ref="G15" si="4">IF(F15&lt;0,CONCATENATE("public static RequestReturnObject ",B15,"(HTTPRequestHeaders oH, string sid)",CHAR(13),"{",CHAR(13),"return com.SendGenericRequest(oH, sid, CMD_",B15,");",CHAR(13),"}",CHAR(13)),"")</f>
         <v>public static RequestReturnObject getTuanGouInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getTuanGouInfo);_x000D_}_x000D_</v>
       </c>
@@ -2400,7 +2392,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G16" s="3" t="str">
+      <c r="G16" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getTuanGouOpenInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getTuanGouOpenInfo);_x000D_}_x000D_</v>
       </c>
@@ -2423,7 +2415,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G17" s="3" t="str">
+      <c r="G17" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject serverOpenTime(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_serverOpenTime);_x000D_}_x000D_</v>
       </c>
@@ -2446,7 +2438,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G18" s="3" t="str">
+      <c r="G18" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject showIconForServerOpenActivity(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_showIconForServerOpenActivity);_x000D_}_x000D_</v>
       </c>
@@ -2469,7 +2461,7 @@
         <f t="shared" ref="F19" si="5">IFERROR(FIND("body",E19),-1)</f>
         <v>83</v>
       </c>
-      <c r="G19" s="3" t="str">
+      <c r="G19" s="1" t="str">
         <f t="shared" ref="G19" si="6">IF(F19&lt;0,CONCATENATE("public static RequestReturnObject ",B19,"(HTTPRequestHeaders oH, string sid)",CHAR(13),"{",CHAR(13),"return com.SendGenericRequest(oH, sid, CMD_",B19,");",CHAR(13),"}",CHAR(13)),"")</f>
         <v/>
       </c>
@@ -2492,7 +2484,7 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="G20" s="3" t="str">
+      <c r="G20" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2515,7 +2507,7 @@
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="G21" s="3" t="str">
+      <c r="G21" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2538,7 +2530,7 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="G22" s="3" t="str">
+      <c r="G22" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2561,7 +2553,7 @@
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="G23" s="3" t="str">
+      <c r="G23" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2584,191 +2576,191 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="G24" s="3" t="str">
+      <c r="G24" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="C25" s="3" t="str">
+      <c r="C25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>private const string CMD_acceptRankReward = "Arena.acceptRankReward";</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="2">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G25" s="3" t="str">
+      <c r="G25" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject acceptRankReward(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_acceptRankReward);_x000D_}_x000D_</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="C26" s="3" t="str">
+      <c r="C26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>private const string CMD_changeEnemies = "Arena.changeEnemies";</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="2">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G26" s="3" t="str">
+      <c r="G26" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject changeEnemies(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_changeEnemies);_x000D_}_x000D_</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="C27" s="3" t="str">
+      <c r="C27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>private const string CMD_getDefFormation = "Arena.getDefFormation";</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="2">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G27" s="3" t="str">
+      <c r="G27" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getDefFormation(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getDefFormation);_x000D_}_x000D_</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="C28" s="3" t="str">
+      <c r="C28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>private const string CMD_myArenaStatus = "Arena.myArenaStatus";</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="2">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G28" s="3" t="str">
+      <c r="G28" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject myArenaStatus(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_myArenaStatus);_x000D_}_x000D_</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="C29" s="3" t="str">
+      <c r="C29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>private const string CMD_changeEnemies = "Arenas.changeEnemies";</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="2">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G29" s="3" t="str">
+      <c r="G29" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject changeEnemies(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_changeEnemies);_x000D_}_x000D_</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="C30" s="3" t="str">
+      <c r="C30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>private const string CMD_drawTimeReward = "Arenas.drawTimeReward";</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="2">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G30" s="3" t="str">
+      <c r="G30" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject drawTimeReward(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_drawTimeReward);_x000D_}_x000D_</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="C31" s="3" t="str">
+      <c r="C31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>private const string CMD_getDefFormation = "Arenas.getDefFormation";</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="2">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G31" s="3" t="str">
+      <c r="G31" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getDefFormation(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getDefFormation);_x000D_}_x000D_</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="C32" s="3" t="str">
+      <c r="C32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>private const string CMD_myArenasStatus = "Arenas.myArenasStatus";</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="2">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G32" s="3" t="str">
+      <c r="G32" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject myArenasStatus(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_myArenasStatus);_x000D_}_x000D_</v>
       </c>
@@ -2791,7 +2783,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G33" s="3" t="str">
+      <c r="G33" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getBagInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getBagInfo);_x000D_}_x000D_</v>
       </c>
@@ -2814,7 +2806,7 @@
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="G34" s="3" t="str">
+      <c r="G34" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -2837,7 +2829,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G35" s="3" t="str">
+      <c r="G35" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getTimeInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getTimeInfo);_x000D_}_x000D_</v>
       </c>
@@ -2860,7 +2852,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G36" s="3" t="str">
+      <c r="G36" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject bossInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_bossInfo);_x000D_}_x000D_</v>
       </c>
@@ -2883,7 +2875,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G37" s="3" t="str">
+      <c r="G37" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject bossLineup(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_bossLineup);_x000D_}_x000D_</v>
       </c>
@@ -2906,7 +2898,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G38" s="3" t="str">
+      <c r="G38" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject enterWar(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_enterWar);_x000D_}_x000D_</v>
       </c>
@@ -2929,7 +2921,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G39" s="3" t="str">
+      <c r="G39" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject keyKillInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_keyKillInfo);_x000D_}_x000D_</v>
       </c>
@@ -2952,7 +2944,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G40" s="3" t="str">
+      <c r="G40" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject leaveWar(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_leaveWar);_x000D_}_x000D_</v>
       </c>
@@ -2975,7 +2967,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G41" s="3" t="str">
+      <c r="G41" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject openInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_openInfo);_x000D_}_x000D_</v>
       </c>
@@ -2998,7 +2990,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G42" s="3" t="str">
+      <c r="G42" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject pk(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_pk);_x000D_}_x000D_</v>
       </c>
@@ -3021,7 +3013,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G43" s="3" t="str">
+      <c r="G43" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject rankInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_rankInfo);_x000D_}_x000D_</v>
       </c>
@@ -3044,7 +3036,7 @@
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="G44" s="3" t="str">
+      <c r="G44" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3067,7 +3059,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G45" s="3" t="str">
+      <c r="G45" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject eliteBuyTime(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_eliteBuyTime);_x000D_}_x000D_</v>
       </c>
@@ -3090,7 +3082,7 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="G46" s="3" t="str">
+      <c r="G46" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3113,7 +3105,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G47" s="3" t="str">
+      <c r="G47" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject eliteGetAllInfos(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_eliteGetAllInfos);_x000D_}_x000D_</v>
       </c>
@@ -3136,7 +3128,7 @@
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="G48" s="3" t="str">
+      <c r="G48" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3159,7 +3151,7 @@
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="G49" s="3" t="str">
+      <c r="G49" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3182,7 +3174,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G50" s="3" t="str">
+      <c r="G50" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject fightNext(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_fightNext);_x000D_}_x000D_</v>
       </c>
@@ -3205,7 +3197,7 @@
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="G51" s="3" t="str">
+      <c r="G51" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3228,7 +3220,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G52" s="3" t="str">
+      <c r="G52" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getLeftTimes(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getLeftTimes);_x000D_}_x000D_</v>
       </c>
@@ -3251,7 +3243,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G53" s="3" t="str">
+      <c r="G53" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getTrialsInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getTrialsInfo);_x000D_}_x000D_</v>
       </c>
@@ -3274,7 +3266,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G54" s="3" t="str">
+      <c r="G54" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject nextEnemies(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_nextEnemies);_x000D_}_x000D_</v>
       </c>
@@ -3297,7 +3289,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G55" s="3" t="str">
+      <c r="G55" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject quitCampaign(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_quitCampaign);_x000D_}_x000D_</v>
       </c>
@@ -3320,7 +3312,7 @@
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="G56" s="3" t="str">
+      <c r="G56" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3343,7 +3335,7 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="G57" s="3" t="str">
+      <c r="G57" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3366,7 +3358,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G58" s="3" t="str">
+      <c r="G58" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject time(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_time);_x000D_}_x000D_</v>
       </c>
@@ -3389,7 +3381,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G59" s="3" t="str">
+      <c r="G59" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject challenge(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_challenge);_x000D_}_x000D_</v>
       </c>
@@ -3412,7 +3404,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G60" s="3" t="str">
+      <c r="G60" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject drawPassRewards(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_drawPassRewards);_x000D_}_x000D_</v>
       </c>
@@ -3435,7 +3427,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G61" s="3" t="str">
+      <c r="G61" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getHuarongRoadInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getHuarongRoadInfo);_x000D_}_x000D_</v>
       </c>
@@ -3458,7 +3450,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G62" s="3" t="str">
+      <c r="G62" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject restartHuarongRoad(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_restartHuarongRoad);_x000D_}_x000D_</v>
       </c>
@@ -3481,7 +3473,7 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="G63" s="3" t="str">
+      <c r="G63" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3504,7 +3496,7 @@
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="G64" s="3" t="str">
+      <c r="G64" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3527,7 +3519,7 @@
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="G65" s="3" t="str">
+      <c r="G65" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3550,7 +3542,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G66" s="3" t="str">
+      <c r="G66" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getPlayerCityInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getPlayerCityInfo);_x000D_}_x000D_</v>
       </c>
@@ -3573,7 +3565,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G67" s="3" t="str">
+      <c r="G67" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject corpsCityReward(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_corpsCityReward);_x000D_}_x000D_</v>
       </c>
@@ -3596,7 +3588,7 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="G68" s="3" t="str">
+      <c r="G68" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3619,7 +3611,7 @@
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="G69" s="3" t="str">
+      <c r="G69" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3642,7 +3634,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G70" s="3" t="str">
+      <c r="G70" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getCorpsMessageNum(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getCorpsMessageNum);_x000D_}_x000D_</v>
       </c>
@@ -3665,7 +3657,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G71" s="3" t="str">
+      <c r="G71" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject getJoinedCorps(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getJoinedCorps);_x000D_}_x000D_</v>
       </c>
@@ -3688,7 +3680,7 @@
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="G72" s="3" t="str">
+      <c r="G72" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3711,7 +3703,7 @@
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="G73" s="3" t="str">
+      <c r="G73" s="1" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3734,7 +3726,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G74" s="3" t="str">
+      <c r="G74" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject personIndustryRefresh(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_personIndustryRefresh);_x000D_}_x000D_</v>
       </c>
@@ -3757,7 +3749,7 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="G75" s="3" t="str">
+      <c r="G75" s="1" t="str">
         <f t="shared" si="2"/>
         <v>public static RequestReturnObject playerTech(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_playerTech);_x000D_}_x000D_</v>
       </c>
@@ -3780,7 +3772,7 @@
         <f t="shared" ref="F76:F139" si="7">IFERROR(FIND("body",E76),-1)</f>
         <v>-1</v>
       </c>
-      <c r="G76" s="3" t="str">
+      <c r="G76" s="1" t="str">
         <f t="shared" ref="G76:G139" si="8">IF(F76&lt;0,CONCATENATE("public static RequestReturnObject ",B76,"(HTTPRequestHeaders oH, string sid)",CHAR(13),"{",CHAR(13),"return com.SendGenericRequest(oH, sid, CMD_",B76,");",CHAR(13),"}",CHAR(13)),"")</f>
         <v>public static RequestReturnObject takeZhanjiStep(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_takeZhanjiStep);_x000D_}_x000D_</v>
       </c>
@@ -3803,7 +3795,7 @@
         <f t="shared" si="7"/>
         <v>85</v>
       </c>
-      <c r="G77" s="3" t="str">
+      <c r="G77" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -3826,7 +3818,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G78" s="3" t="str">
+      <c r="G78" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getInfo);_x000D_}_x000D_</v>
       </c>
@@ -3849,7 +3841,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G79" s="3" t="str">
+      <c r="G79" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject corpsCountry(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_corpsCountry);_x000D_}_x000D_</v>
       </c>
@@ -3872,7 +3864,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G80" s="3" t="str">
+      <c r="G80" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject viewCountry(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_viewCountry);_x000D_}_x000D_</v>
       </c>
@@ -3895,7 +3887,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G81" s="3" t="str">
+      <c r="G81" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getInfo);_x000D_}_x000D_</v>
       </c>
@@ -3918,7 +3910,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G82" s="3" t="str">
+      <c r="G82" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getJackpotInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getJackpotInfo);_x000D_}_x000D_</v>
       </c>
@@ -3941,7 +3933,7 @@
         <f t="shared" si="7"/>
         <v>96</v>
       </c>
-      <c r="G83" s="3" t="str">
+      <c r="G83" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -3964,7 +3956,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G84" s="3" t="str">
+      <c r="G84" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getDramaInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getDramaInfo);_x000D_}_x000D_</v>
       </c>
@@ -3987,7 +3979,7 @@
         <f t="shared" si="7"/>
         <v>82</v>
       </c>
-      <c r="G85" s="3" t="str">
+      <c r="G85" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4010,7 +4002,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G86" s="3" t="str">
+      <c r="G86" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getInfo);_x000D_}_x000D_</v>
       </c>
@@ -4033,7 +4025,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G87" s="3" t="str">
+      <c r="G87" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject open(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_open);_x000D_}_x000D_</v>
       </c>
@@ -4056,7 +4048,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G88" s="3" t="str">
+      <c r="G88" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject openBox(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_openBox);_x000D_}_x000D_</v>
       </c>
@@ -4079,7 +4071,7 @@
         <f t="shared" si="7"/>
         <v>81</v>
       </c>
-      <c r="G89" s="3" t="str">
+      <c r="G89" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4102,7 +4094,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G90" s="3" t="str">
+      <c r="G90" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject openInBox(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_openInBox);_x000D_}_x000D_</v>
       </c>
@@ -4125,7 +4117,7 @@
         <f t="shared" si="7"/>
         <v>72</v>
       </c>
-      <c r="G91" s="3" t="str">
+      <c r="G91" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4148,7 +4140,7 @@
         <f t="shared" si="7"/>
         <v>77</v>
       </c>
-      <c r="G92" s="3" t="str">
+      <c r="G92" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4171,7 +4163,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G93" s="3" t="str">
+      <c r="G93" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject collected(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_collected);_x000D_}_x000D_</v>
       </c>
@@ -4194,7 +4186,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G94" s="3" t="str">
+      <c r="G94" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject draw(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_draw);_x000D_}_x000D_</v>
       </c>
@@ -4217,7 +4209,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G95" s="3" t="str">
+      <c r="G95" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getBuyInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getBuyInfo);_x000D_}_x000D_</v>
       </c>
@@ -4240,7 +4232,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G96" s="3" t="str">
+      <c r="G96" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getGameInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getGameInfo);_x000D_}_x000D_</v>
       </c>
@@ -4263,7 +4255,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G97" s="3" t="str">
+      <c r="G97" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject isFloat(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_isFloat);_x000D_}_x000D_</v>
       </c>
@@ -4286,7 +4278,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G98" s="3" t="str">
+      <c r="G98" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject activityInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_activityInfo);_x000D_}_x000D_</v>
       </c>
@@ -4309,7 +4301,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G99" s="3" t="str">
+      <c r="G99" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject myFirecrackerInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_myFirecrackerInfo);_x000D_}_x000D_</v>
       </c>
@@ -4332,7 +4324,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G100" s="3" t="str">
+      <c r="G100" s="1" t="str">
         <f>IF(F100&lt;0,CONCATENATE("public static RequestReturnObject ",B100,"(HTTPRequestHeaders oH, string sid)",CHAR(13),"{",CHAR(13),"return com.SendGenericRequest(oH, sid, CMD_",B100,");",CHAR(13),"}",CHAR(13)),"")</f>
         <v>public static RequestReturnObject chouqianOpenInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_chouqianOpenInfo);_x000D_}_x000D_</v>
       </c>
@@ -4355,7 +4347,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G101" s="3" t="str">
+      <c r="G101" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject superPackageInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_superPackageInfo);_x000D_}_x000D_</v>
       </c>
@@ -4378,7 +4370,7 @@
         <f t="shared" si="7"/>
         <v>79</v>
       </c>
-      <c r="G102" s="3" t="str">
+      <c r="G102" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4401,7 +4393,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G103" s="3" t="str">
+      <c r="G103" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject godStrenInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_godStrenInfo);_x000D_}_x000D_</v>
       </c>
@@ -4424,7 +4416,7 @@
         <f t="shared" si="7"/>
         <v>83</v>
       </c>
-      <c r="G104" s="3" t="str">
+      <c r="G104" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4447,7 +4439,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G105" s="3" t="str">
+      <c r="G105" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject acquireGrassArrowInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_acquireGrassArrowInfo);_x000D_}_x000D_</v>
       </c>
@@ -4470,7 +4462,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G106" s="3" t="str">
+      <c r="G106" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject doGrassArrowFight(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_doGrassArrowFight);_x000D_}_x000D_</v>
       </c>
@@ -4493,7 +4485,7 @@
         <f t="shared" si="7"/>
         <v>88</v>
       </c>
-      <c r="G107" s="3" t="str">
+      <c r="G107" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4516,7 +4508,7 @@
         <f t="shared" si="7"/>
         <v>91</v>
       </c>
-      <c r="G108" s="3" t="str">
+      <c r="G108" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4539,7 +4531,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G109" s="3" t="str">
+      <c r="G109" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject assessScore(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_assessScore);_x000D_}_x000D_</v>
       </c>
@@ -4562,7 +4554,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G110" s="3" t="str">
+      <c r="G110" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getConvenientFormations(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getConvenientFormations);_x000D_}_x000D_</v>
       </c>
@@ -4585,7 +4577,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G111" s="3" t="str">
+      <c r="G111" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getCurrRecommendActivityInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getCurrRecommendActivityInfo);_x000D_}_x000D_</v>
       </c>
@@ -4608,7 +4600,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G112" s="3" t="str">
+      <c r="G112" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getFeastInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getFeastInfo);_x000D_}_x000D_</v>
       </c>
@@ -4631,7 +4623,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G113" s="3" t="str">
+      <c r="G113" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getHeroIconInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getHeroIconInfo);_x000D_}_x000D_</v>
       </c>
@@ -4654,7 +4646,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G114" s="3" t="str">
+      <c r="G114" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getPlayerHeroList(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getPlayerHeroList);_x000D_}_x000D_</v>
       </c>
@@ -4677,7 +4669,7 @@
         <f t="shared" si="7"/>
         <v>79</v>
       </c>
-      <c r="G115" s="3" t="str">
+      <c r="G115" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4700,7 +4692,7 @@
         <f t="shared" si="7"/>
         <v>83</v>
       </c>
-      <c r="G116" s="3" t="str">
+      <c r="G116" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4723,7 +4715,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G117" s="3" t="str">
+      <c r="G117" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getWineInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getWineInfo);_x000D_}_x000D_</v>
       </c>
@@ -4746,7 +4738,7 @@
         <f t="shared" si="7"/>
         <v>76</v>
       </c>
-      <c r="G118" s="3" t="str">
+      <c r="G118" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4769,7 +4761,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G119" s="3" t="str">
+      <c r="G119" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject afterSeasonEnemy(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_afterSeasonEnemy);_x000D_}_x000D_</v>
       </c>
@@ -4792,7 +4784,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G120" s="3" t="str">
+      <c r="G120" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject kingroadEnd(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_kingroadEnd);_x000D_}_x000D_</v>
       </c>
@@ -4815,7 +4807,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G121" s="3" t="str">
+      <c r="G121" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject kingroadState(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_kingroadState);_x000D_}_x000D_</v>
       </c>
@@ -4838,7 +4830,7 @@
         <f t="shared" si="7"/>
         <v>86</v>
       </c>
-      <c r="G122" s="3" t="str">
+      <c r="G122" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4861,7 +4853,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G123" s="3" t="str">
+      <c r="G123" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getOfflineConpensate(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getOfflineConpensate);_x000D_}_x000D_</v>
       </c>
@@ -4884,7 +4876,7 @@
         <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="G124" s="3" t="str">
+      <c r="G124" s="1" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
@@ -4907,7 +4899,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G125" s="3" t="str">
+      <c r="G125" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject loginFinish(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_loginFinish);_x000D_}_x000D_</v>
       </c>
@@ -4930,7 +4922,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G126" s="3" t="str">
+      <c r="G126" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject serverInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_serverInfo);_x000D_}_x000D_</v>
       </c>
@@ -4953,7 +4945,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G127" s="3" t="str">
+      <c r="G127" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getBuyResetTimes(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getBuyResetTimes);_x000D_}_x000D_</v>
       </c>
@@ -4976,7 +4968,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G128" s="3" t="str">
+      <c r="G128" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getFinishedReward(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getFinishedReward);_x000D_}_x000D_</v>
       </c>
@@ -4999,7 +4991,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G129" s="3" t="str">
+      <c r="G129" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getHeroStatus(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getHeroStatus);_x000D_}_x000D_</v>
       </c>
@@ -5022,7 +5014,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G130" s="3" t="str">
+      <c r="G130" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getMyStatus(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getMyStatus);_x000D_}_x000D_</v>
       </c>
@@ -5045,7 +5037,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G131" s="3" t="str">
+      <c r="G131" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getUnpassBuff(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getUnpassBuff);_x000D_}_x000D_</v>
       </c>
@@ -5068,7 +5060,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G132" s="3" t="str">
+      <c r="G132" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject restart(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_restart);_x000D_}_x000D_</v>
       </c>
@@ -5091,7 +5083,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G133" s="3" t="str">
+      <c r="G133" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject getDispInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getDispInfo);_x000D_}_x000D_</v>
       </c>
@@ -5114,7 +5106,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G134" s="3" t="str">
+      <c r="G134" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject drawLottery(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_drawLottery);_x000D_}_x000D_</v>
       </c>
@@ -5137,7 +5129,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G135" s="3" t="str">
+      <c r="G135" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject freeLottery(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_freeLottery);_x000D_}_x000D_</v>
       </c>
@@ -5160,7 +5152,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G136" s="3" t="str">
+      <c r="G136" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject openLottery(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_openLottery);_x000D_}_x000D_</v>
       </c>
@@ -5183,7 +5175,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G137" s="3" t="str">
+      <c r="G137" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject refreshLottery(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_refreshLottery);_x000D_}_x000D_</v>
       </c>
@@ -5206,7 +5198,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G138" s="3" t="str">
+      <c r="G138" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject draw(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_draw);_x000D_}_x000D_</v>
       </c>
@@ -5229,7 +5221,7 @@
         <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="G139" s="3" t="str">
+      <c r="G139" s="1" t="str">
         <f t="shared" si="8"/>
         <v>public static RequestReturnObject info(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_info);_x000D_}_x000D_</v>
       </c>
@@ -5252,7 +5244,7 @@
         <f t="shared" ref="F140:F203" si="10">IFERROR(FIND("body",E140),-1)</f>
         <v>-1</v>
       </c>
-      <c r="G140" s="3" t="str">
+      <c r="G140" s="1" t="str">
         <f t="shared" ref="G140:G203" si="11">IF(F140&lt;0,CONCATENATE("public static RequestReturnObject ",B140,"(HTTPRequestHeaders oH, string sid)",CHAR(13),"{",CHAR(13),"return com.SendGenericRequest(oH, sid, CMD_",B140,");",CHAR(13),"}",CHAR(13)),"")</f>
         <v>public static RequestReturnObject getMyMajorInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getMyMajorInfo);_x000D_}_x000D_</v>
       </c>
@@ -5275,7 +5267,7 @@
         <f t="shared" si="10"/>
         <v>79</v>
       </c>
-      <c r="G141" s="3" t="str">
+      <c r="G141" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5298,7 +5290,7 @@
         <f t="shared" si="10"/>
         <v>79</v>
       </c>
-      <c r="G142" s="3" t="str">
+      <c r="G142" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5321,7 +5313,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G143" s="3" t="str">
+      <c r="G143" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject armsTechnology(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_armsTechnology);_x000D_}_x000D_</v>
       </c>
@@ -5344,7 +5336,7 @@
         <f t="shared" si="10"/>
         <v>79</v>
       </c>
-      <c r="G144" s="3" t="str">
+      <c r="G144" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5367,7 +5359,7 @@
         <f t="shared" si="10"/>
         <v>81</v>
       </c>
-      <c r="G145" s="3" t="str">
+      <c r="G145" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5390,7 +5382,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G146" s="3" t="str">
+      <c r="G146" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject decreeInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_decreeInfo);_x000D_}_x000D_</v>
       </c>
@@ -5413,7 +5405,7 @@
         <f t="shared" si="10"/>
         <v>82</v>
       </c>
-      <c r="G147" s="3" t="str">
+      <c r="G147" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5436,7 +5428,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G148" s="3" t="str">
+      <c r="G148" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getManorInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getManorInfo);_x000D_}_x000D_</v>
       </c>
@@ -5459,7 +5451,7 @@
         <f t="shared" si="10"/>
         <v>83</v>
       </c>
-      <c r="G149" s="3" t="str">
+      <c r="G149" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5482,7 +5474,7 @@
         <f t="shared" si="10"/>
         <v>82</v>
       </c>
-      <c r="G150" s="3" t="str">
+      <c r="G150" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5505,7 +5497,7 @@
         <f t="shared" si="10"/>
         <v>81</v>
       </c>
-      <c r="G151" s="3" t="str">
+      <c r="G151" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5528,7 +5520,7 @@
         <f t="shared" si="10"/>
         <v>80</v>
       </c>
-      <c r="G152" s="3" t="str">
+      <c r="G152" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5551,7 +5543,7 @@
         <f t="shared" si="10"/>
         <v>87</v>
       </c>
-      <c r="G153" s="3" t="str">
+      <c r="G153" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5574,7 +5566,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G154" s="3" t="str">
+      <c r="G154" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject refreshManor(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_refreshManor);_x000D_}_x000D_</v>
       </c>
@@ -5597,7 +5589,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G155" s="3" t="str">
+      <c r="G155" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject resHourOutput(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_resHourOutput);_x000D_}_x000D_</v>
       </c>
@@ -5620,7 +5612,7 @@
         <f t="shared" si="10"/>
         <v>77</v>
       </c>
-      <c r="G156" s="3" t="str">
+      <c r="G156" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5643,7 +5635,7 @@
         <f t="shared" si="10"/>
         <v>81</v>
       </c>
-      <c r="G157" s="3" t="str">
+      <c r="G157" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5666,7 +5658,7 @@
         <f t="shared" si="10"/>
         <v>89</v>
       </c>
-      <c r="G158" s="3" t="str">
+      <c r="G158" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5689,7 +5681,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G159" s="3" t="str">
+      <c r="G159" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getOpenInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getOpenInfo);_x000D_}_x000D_</v>
       </c>
@@ -5712,7 +5704,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G160" s="3" t="str">
+      <c r="G160" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject acquireCityCommandInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_acquireCityCommandInfo);_x000D_}_x000D_</v>
       </c>
@@ -5735,7 +5727,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G161" s="3" t="str">
+      <c r="G161" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject acquireNationCardPanelInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_acquireNationCardPanelInfo);_x000D_}_x000D_</v>
       </c>
@@ -5758,7 +5750,7 @@
         <f t="shared" si="10"/>
         <v>89</v>
       </c>
-      <c r="G162" s="3" t="str">
+      <c r="G162" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5781,7 +5773,7 @@
         <f t="shared" si="10"/>
         <v>97</v>
       </c>
-      <c r="G163" s="3" t="str">
+      <c r="G163" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5804,7 +5796,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G164" s="3" t="str">
+      <c r="G164" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getMyTroops(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getMyTroops);_x000D_}_x000D_</v>
       </c>
@@ -5827,7 +5819,7 @@
         <f t="shared" si="10"/>
         <v>76</v>
       </c>
-      <c r="G165" s="3" t="str">
+      <c r="G165" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5850,7 +5842,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G166" s="3" t="str">
+      <c r="G166" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getInfo);_x000D_}_x000D_</v>
       </c>
@@ -5873,7 +5865,7 @@
         <f t="shared" si="10"/>
         <v>82</v>
       </c>
-      <c r="G167" s="3" t="str">
+      <c r="G167" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5896,7 +5888,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G168" s="3" t="str">
+      <c r="G168" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject inMissionHeros(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_inMissionHeros);_x000D_}_x000D_</v>
       </c>
@@ -5919,7 +5911,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G169" s="3" t="str">
+      <c r="G169" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject killRank(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_killRank);_x000D_}_x000D_</v>
       </c>
@@ -5942,7 +5934,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G170" s="3" t="str">
+      <c r="G170" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject leaveWar(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_leaveWar);_x000D_}_x000D_</v>
       </c>
@@ -5965,7 +5957,7 @@
         <f t="shared" si="10"/>
         <v>84</v>
       </c>
-      <c r="G171" s="3" t="str">
+      <c r="G171" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -5988,7 +5980,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G172" s="3" t="str">
+      <c r="G172" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject rewardCfg(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_rewardCfg);_x000D_}_x000D_</v>
       </c>
@@ -6011,7 +6003,7 @@
         <f t="shared" si="10"/>
         <v>78</v>
       </c>
-      <c r="G173" s="3" t="str">
+      <c r="G173" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -6034,7 +6026,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G174" s="3" t="str">
+      <c r="G174" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject enterWar(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_enterWar);_x000D_}_x000D_</v>
       </c>
@@ -6057,7 +6049,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G175" s="3" t="str">
+      <c r="G175" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject inMissionHeros(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_inMissionHeros);_x000D_}_x000D_</v>
       </c>
@@ -6080,7 +6072,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G176" s="3" t="str">
+      <c r="G176" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject leaveWar(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_leaveWar);_x000D_}_x000D_</v>
       </c>
@@ -6103,7 +6095,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G177" s="3" t="str">
+      <c r="G177" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject northCitySituation(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_northCitySituation);_x000D_}_x000D_</v>
       </c>
@@ -6126,7 +6118,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G178" s="3" t="str">
+      <c r="G178" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject retreatAllTroops(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_retreatAllTroops);_x000D_}_x000D_</v>
       </c>
@@ -6149,7 +6141,7 @@
         <f t="shared" si="10"/>
         <v>82</v>
       </c>
-      <c r="G179" s="3" t="str">
+      <c r="G179" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -6172,7 +6164,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G180" s="3" t="str">
+      <c r="G180" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject queryAllMarqueeMessage(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_queryAllMarqueeMessage);_x000D_}_x000D_</v>
       </c>
@@ -6195,7 +6187,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G181" s="3" t="str">
+      <c r="G181" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getNpcWars(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getNpcWars);_x000D_}_x000D_</v>
       </c>
@@ -6218,7 +6210,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G182" s="3" t="str">
+      <c r="G182" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject cityStatus(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_cityStatus);_x000D_}_x000D_</v>
       </c>
@@ -6241,7 +6233,7 @@
         <f t="shared" si="10"/>
         <v>86</v>
       </c>
-      <c r="G183" s="3" t="str">
+      <c r="G183" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -6264,7 +6256,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G184" s="3" t="str">
+      <c r="G184" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getPatrolInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getPatrolInfo);_x000D_}_x000D_</v>
       </c>
@@ -6287,7 +6279,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G185" s="3" t="str">
+      <c r="G185" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getPlatformInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getPlatformInfo);_x000D_}_x000D_</v>
       </c>
@@ -6310,7 +6302,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G186" s="3" t="str">
+      <c r="G186" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getProperties(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getProperties);_x000D_}_x000D_</v>
       </c>
@@ -6333,7 +6325,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G187" s="3" t="str">
+      <c r="G187" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getSpecialState(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getSpecialState);_x000D_}_x000D_</v>
       </c>
@@ -6356,7 +6348,7 @@
         <f t="shared" si="10"/>
         <v>88</v>
       </c>
-      <c r="G188" s="3" t="str">
+      <c r="G188" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -6379,7 +6371,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G189" s="3" t="str">
+      <c r="G189" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getPrayTime(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getPrayTime);_x000D_}_x000D_</v>
       </c>
@@ -6402,7 +6394,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G190" s="3" t="str">
+      <c r="G190" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject findAllPowerRank(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_findAllPowerRank);_x000D_}_x000D_</v>
       </c>
@@ -6425,7 +6417,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G191" s="3" t="str">
+      <c r="G191" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject activityTime(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_activityTime);_x000D_}_x000D_</v>
       </c>
@@ -6448,7 +6440,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G192" s="3" t="str">
+      <c r="G192" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getSevenDayFundRewardInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getSevenDayFundRewardInfo);_x000D_}_x000D_</v>
       </c>
@@ -6471,7 +6463,7 @@
         <f t="shared" si="10"/>
         <v>86</v>
       </c>
-      <c r="G193" s="3" t="str">
+      <c r="G193" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -6494,7 +6486,7 @@
         <f t="shared" si="10"/>
         <v>81</v>
       </c>
-      <c r="G194" s="3" t="str">
+      <c r="G194" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -6517,7 +6509,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G195" s="3" t="str">
+      <c r="G195" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject availableShops(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_availableShops);_x000D_}_x000D_</v>
       </c>
@@ -6540,7 +6532,7 @@
         <f t="shared" si="10"/>
         <v>83</v>
       </c>
-      <c r="G196" s="3" t="str">
+      <c r="G196" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -6563,7 +6555,7 @@
         <f t="shared" si="10"/>
         <v>78</v>
       </c>
-      <c r="G197" s="3" t="str">
+      <c r="G197" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -6586,7 +6578,7 @@
         <f t="shared" si="10"/>
         <v>84</v>
       </c>
-      <c r="G198" s="3" t="str">
+      <c r="G198" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -6609,7 +6601,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G199" s="3" t="str">
+      <c r="G199" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getCycleShopInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getCycleShopInfo);_x000D_}_x000D_</v>
       </c>
@@ -6632,7 +6624,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G200" s="3" t="str">
+      <c r="G200" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getResourceTradeInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getResourceTradeInfo);_x000D_}_x000D_</v>
       </c>
@@ -6655,7 +6647,7 @@
         <f t="shared" si="10"/>
         <v>78</v>
       </c>
-      <c r="G201" s="3" t="str">
+      <c r="G201" s="1" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
@@ -6678,7 +6670,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G202" s="3" t="str">
+      <c r="G202" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getShuangShiyiShopInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getShuangShiyiShopInfo);_x000D_}_x000D_</v>
       </c>
@@ -6701,7 +6693,7 @@
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="G203" s="3" t="str">
+      <c r="G203" s="1" t="str">
         <f t="shared" si="11"/>
         <v>public static RequestReturnObject getTravelShopInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getTravelShopInfo);_x000D_}_x000D_</v>
       </c>
@@ -6724,7 +6716,7 @@
         <f t="shared" ref="F204:F248" si="13">IFERROR(FIND("body",E204),-1)</f>
         <v>-1</v>
       </c>
-      <c r="G204" s="3" t="str">
+      <c r="G204" s="1" t="str">
         <f t="shared" ref="G204:G248" si="14">IF(F204&lt;0,CONCATENATE("public static RequestReturnObject ",B204,"(HTTPRequestHeaders oH, string sid)",CHAR(13),"{",CHAR(13),"return com.SendGenericRequest(oH, sid, CMD_",B204,");",CHAR(13),"}",CHAR(13)),"")</f>
         <v>public static RequestReturnObject otherShopsRefreshTime(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_otherShopsRefreshTime);_x000D_}_x000D_</v>
       </c>
@@ -6747,7 +6739,7 @@
         <f t="shared" si="13"/>
         <v>78</v>
       </c>
-      <c r="G205" s="3" t="str">
+      <c r="G205" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -6770,7 +6762,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G206" s="3" t="str">
+      <c r="G206" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject shopNextRefreshTime(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_shopNextRefreshTime);_x000D_}_x000D_</v>
       </c>
@@ -6793,7 +6785,7 @@
         <f t="shared" si="13"/>
         <v>80</v>
       </c>
-      <c r="G207" s="3" t="str">
+      <c r="G207" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -6816,7 +6808,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G208" s="3" t="str">
+      <c r="G208" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject availableShops(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_availableShops);_x000D_}_x000D_</v>
       </c>
@@ -6839,7 +6831,7 @@
         <f t="shared" si="13"/>
         <v>75</v>
       </c>
-      <c r="G209" s="3" t="str">
+      <c r="G209" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -6862,7 +6854,7 @@
         <f t="shared" si="13"/>
         <v>77</v>
       </c>
-      <c r="G210" s="3" t="str">
+      <c r="G210" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -6885,7 +6877,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G211" s="3" t="str">
+      <c r="G211" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getInfo);_x000D_}_x000D_</v>
       </c>
@@ -6908,7 +6900,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G212" s="3" t="str">
+      <c r="G212" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject signIn(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_signIn);_x000D_}_x000D_</v>
       </c>
@@ -6931,7 +6923,7 @@
         <f t="shared" si="13"/>
         <v>89</v>
       </c>
-      <c r="G213" s="3" t="str">
+      <c r="G213" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -6954,7 +6946,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G214" s="3" t="str">
+      <c r="G214" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject activityInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_activityInfo);_x000D_}_x000D_</v>
       </c>
@@ -6977,7 +6969,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G215" s="3" t="str">
+      <c r="G215" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject myFirecrackerInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_myFirecrackerInfo);_x000D_}_x000D_</v>
       </c>
@@ -7000,7 +6992,7 @@
         <f t="shared" si="13"/>
         <v>73</v>
       </c>
-      <c r="G216" s="3" t="str">
+      <c r="G216" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7023,7 +7015,7 @@
         <f t="shared" si="13"/>
         <v>77</v>
       </c>
-      <c r="G217" s="3" t="str">
+      <c r="G217" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7046,7 +7038,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G218" s="3" t="str">
+      <c r="G218" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getAchievementInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getAchievementInfo);_x000D_}_x000D_</v>
       </c>
@@ -7069,7 +7061,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G219" s="3" t="str">
+      <c r="G219" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getTaskTraceInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getTaskTraceInfo);_x000D_}_x000D_</v>
       </c>
@@ -7092,7 +7084,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G220" s="3" t="str">
+      <c r="G220" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject teamDuplicateFreeTimes(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_teamDuplicateFreeTimes);_x000D_}_x000D_</v>
       </c>
@@ -7115,7 +7107,7 @@
         <f t="shared" si="13"/>
         <v>79</v>
       </c>
-      <c r="G221" s="3" t="str">
+      <c r="G221" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7138,7 +7130,7 @@
         <f t="shared" si="13"/>
         <v>75</v>
       </c>
-      <c r="G222" s="3" t="str">
+      <c r="G222" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7161,7 +7153,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G223" s="3" t="str">
+      <c r="G223" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject checkOut(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_checkOut);_x000D_}_x000D_</v>
       </c>
@@ -7184,7 +7176,7 @@
         <f t="shared" si="13"/>
         <v>80</v>
       </c>
-      <c r="G224" s="3" t="str">
+      <c r="G224" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7207,7 +7199,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G225" s="3" t="str">
+      <c r="G225" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject dice(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_dice);_x000D_}_x000D_</v>
       </c>
@@ -7230,7 +7222,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G226" s="3" t="str">
+      <c r="G226" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject escape(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_escape);_x000D_}_x000D_</v>
       </c>
@@ -7253,7 +7245,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G227" s="3" t="str">
+      <c r="G227" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getMapInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getMapInfo);_x000D_}_x000D_</v>
       </c>
@@ -7276,7 +7268,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G228" s="3" t="str">
+      <c r="G228" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getStatus(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getStatus);_x000D_}_x000D_</v>
       </c>
@@ -7299,7 +7291,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G229" s="3" t="str">
+      <c r="G229" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject restartTravel(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_restartTravel);_x000D_}_x000D_</v>
       </c>
@@ -7322,7 +7314,7 @@
         <f t="shared" si="13"/>
         <v>77</v>
       </c>
-      <c r="G230" s="3" t="str">
+      <c r="G230" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7345,7 +7337,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G231" s="3" t="str">
+      <c r="G231" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getTurnCardRewards(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getTurnCardRewards);_x000D_}_x000D_</v>
       </c>
@@ -7368,7 +7360,7 @@
         <f t="shared" si="13"/>
         <v>85</v>
       </c>
-      <c r="G232" s="3" t="str">
+      <c r="G232" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7391,7 +7383,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G233" s="3" t="str">
+      <c r="G233" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getActivityInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getActivityInfo);_x000D_}_x000D_</v>
       </c>
@@ -7414,7 +7406,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G234" s="3" t="str">
+      <c r="G234" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject firstChargeInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_firstChargeInfo);_x000D_}_x000D_</v>
       </c>
@@ -7437,7 +7429,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G235" s="3" t="str">
+      <c r="G235" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject monthCard(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_monthCard);_x000D_}_x000D_</v>
       </c>
@@ -7460,7 +7452,7 @@
         <f t="shared" si="13"/>
         <v>83</v>
       </c>
-      <c r="G236" s="3" t="str">
+      <c r="G236" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7483,7 +7475,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G237" s="3" t="str">
+      <c r="G237" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject isGotMobileGift(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_isGotMobileGift);_x000D_}_x000D_</v>
       </c>
@@ -7506,7 +7498,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G238" s="3" t="str">
+      <c r="G238" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject time(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_time);_x000D_}_x000D_</v>
       </c>
@@ -7529,7 +7521,7 @@
         <f t="shared" si="13"/>
         <v>87</v>
       </c>
-      <c r="G239" s="3" t="str">
+      <c r="G239" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7552,7 +7544,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G240" s="3" t="str">
+      <c r="G240" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getAllOpenedCities(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getAllOpenedCities);_x000D_}_x000D_</v>
       </c>
@@ -7575,7 +7567,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G241" s="3" t="str">
+      <c r="G241" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getAllTransportingUnits(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getAllTransportingUnits);_x000D_}_x000D_</v>
       </c>
@@ -7598,7 +7590,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G242" s="3" t="str">
+      <c r="G242" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getCityChapterBlueprint(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getCityChapterBlueprint);_x000D_}_x000D_</v>
       </c>
@@ -7621,7 +7613,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G243" s="3" t="str">
+      <c r="G243" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getCityRewardInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getCityRewardInfo);_x000D_}_x000D_</v>
       </c>
@@ -7644,7 +7636,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G244" s="3" t="str">
+      <c r="G244" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getExploredWorldArea(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getExploredWorldArea);_x000D_}_x000D_</v>
       </c>
@@ -7667,7 +7659,7 @@
         <f t="shared" si="13"/>
         <v>70</v>
       </c>
-      <c r="G245" s="3" t="str">
+      <c r="G245" s="1" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
@@ -7690,7 +7682,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G246" s="3" t="str">
+      <c r="G246" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject worldSituation(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_worldSituation);_x000D_}_x000D_</v>
       </c>
@@ -7713,7 +7705,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G247" s="3" t="str">
+      <c r="G247" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getYunYouInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getYunYouInfo);_x000D_}_x000D_</v>
       </c>
@@ -7736,7 +7728,7 @@
         <f t="shared" si="13"/>
         <v>-1</v>
       </c>
-      <c r="G248" s="3" t="str">
+      <c r="G248" s="1" t="str">
         <f t="shared" si="14"/>
         <v>public static RequestReturnObject getTimeInfo(HTTPRequestHeaders oH, string sid)_x000D_{_x000D_return com.SendGenericRequest(oH, sid, CMD_getTimeInfo);_x000D_}_x000D_</v>
       </c>

</xml_diff>